<commit_message>
Update data package at: 2024-02-08T16:24:45Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1528"/>
+  <dimension ref="A1:H1529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -43470,35 +43470,35 @@
     </row>
     <row r="1283">
       <c r="A1283">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B1283" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS A FUNDOS</t>
+          <t>RECURSOS DE ALIENAÇÃO DE BENS/ATIVOS - ADMINISTRAÇÃO INDIRETA</t>
         </is>
       </c>
       <c r="C1283">
-        <v>4031</v>
+        <v>2251</v>
       </c>
       <c r="D1283" t="inlineStr">
         <is>
-          <t>FEPJ</t>
+          <t>JUCEMG</t>
         </is>
       </c>
       <c r="E1283">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F1283" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>ALIENACAO DE BENS DE ENTIDADES ESTADUAIS</t>
         </is>
       </c>
       <c r="G1283">
-        <v>1611010123003</v>
+        <v>2213010101000</v>
       </c>
       <c r="H1283" t="inlineStr">
         <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - PODER JUDIC. - VERBA INDENIZATORIA DE TRANSPORTE CUSTEADA PELAS PARTES</t>
+          <t>ALIENACAO BENS MOVEIS SEMOVENTES - PRINC.</t>
         </is>
       </c>
     </row>
@@ -43512,27 +43512,27 @@
         </is>
       </c>
       <c r="C1284">
-        <v>4141</v>
+        <v>4031</v>
       </c>
       <c r="D1284" t="inlineStr">
         <is>
-          <t>FPE</t>
+          <t>FEPJ</t>
         </is>
       </c>
       <c r="E1284">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F1284" t="inlineStr">
         <is>
-          <t>MULTAS PECUNIARIAS E JUROS DE MORA FIXADOS EM SENTENCAS JUDICIAIS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1284">
-        <v>1911080101000</v>
+        <v>1611010123003</v>
       </c>
       <c r="H1284" t="inlineStr">
         <is>
-          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
+          <t>SERVICOS ADM. COMERC. GER. - PRINC. - PODER JUDIC. - VERBA INDENIZATORIA DE TRANSPORTE CUSTEADA PELAS PARTES</t>
         </is>
       </c>
     </row>
@@ -43546,27 +43546,27 @@
         </is>
       </c>
       <c r="C1285">
-        <v>4331</v>
+        <v>4141</v>
       </c>
       <c r="D1285" t="inlineStr">
         <is>
-          <t>FDM</t>
+          <t>FPE</t>
         </is>
       </c>
       <c r="E1285">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F1285" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>MULTAS PECUNIARIAS E JUROS DE MORA FIXADOS EM SENTENCAS JUDICIAIS</t>
         </is>
       </c>
       <c r="G1285">
-        <v>1739990111001</v>
+        <v>1911080101000</v>
       </c>
       <c r="H1285" t="inlineStr">
         <is>
-          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
+          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
         </is>
       </c>
     </row>
@@ -43596,11 +43596,11 @@
         </is>
       </c>
       <c r="G1286">
-        <v>1999992299000</v>
+        <v>1739990111001</v>
       </c>
       <c r="H1286" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - MJM - DEMAIS</t>
+          <t>COMERCIO E SERVICOS - DIVERSOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -43614,27 +43614,27 @@
         </is>
       </c>
       <c r="C1287">
-        <v>4341</v>
+        <v>4331</v>
       </c>
       <c r="D1287" t="inlineStr">
         <is>
-          <t>FHIDRO</t>
+          <t>FDM</t>
         </is>
       </c>
       <c r="E1287">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1287" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1287">
-        <v>1911010112000</v>
+        <v>1999992299000</v>
       </c>
       <c r="H1287" t="inlineStr">
         <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - INFRACAO A LEGISLACAO DE ABASTECIMENTO DE AGUA E ESGOTAMENTO SANITARIO</t>
+          <t>OUTRAS REC. - PRIMARIAS - MJM - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -43648,27 +43648,27 @@
         </is>
       </c>
       <c r="C1288">
-        <v>4381</v>
+        <v>4341</v>
       </c>
       <c r="D1288" t="inlineStr">
         <is>
-          <t>FUNTRANS</t>
+          <t>FHIDRO</t>
         </is>
       </c>
       <c r="E1288">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F1288" t="inlineStr">
         <is>
-          <t>TAXA DE LICENCIAMENTO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1288">
-        <v>1121010103000</v>
+        <v>1911010112000</v>
       </c>
       <c r="H1288" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - PRINC. - TAXA DE LICENCIAMENTO PARA USO OU OCUPACAO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
+          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - INFRACAO A LEGISLACAO DE ABASTECIMENTO DE AGUA E ESGOTAMENTO SANITARIO</t>
         </is>
       </c>
     </row>
@@ -43698,11 +43698,11 @@
         </is>
       </c>
       <c r="G1289">
-        <v>1121010203000</v>
+        <v>1121010103000</v>
       </c>
       <c r="H1289" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - MJM - TAXA DE LICENCIAMENTO PARA USO OU OCUPACAO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
+          <t>TX. INSP. CONTR. FISC. - PRINC. - TAXA DE LICENCIAMENTO PARA USO OU OCUPACAO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
         </is>
       </c>
     </row>
@@ -43716,27 +43716,27 @@
         </is>
       </c>
       <c r="C1290">
-        <v>4421</v>
+        <v>4381</v>
       </c>
       <c r="D1290" t="inlineStr">
         <is>
-          <t>FUNDIF</t>
+          <t>FUNTRANS</t>
         </is>
       </c>
       <c r="E1290">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F1290" t="inlineStr">
         <is>
-          <t>MULTAS PECUNIARIAS E JUROS DE MORA FIXADOS EM SENTENCAS JUDICIAIS</t>
+          <t>TAXA DE LICENCIAMENTO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
         </is>
       </c>
       <c r="G1290">
-        <v>1911080101000</v>
+        <v>1121010203000</v>
       </c>
       <c r="H1290" t="inlineStr">
         <is>
-          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
+          <t>TX. INSP. CONTR. FISC. - MJM - TAXA DE LICENCIAMENTO PARA USO OU OCUPACAO DA FAIXA DE DOMINIO DAS RODOVIAS</t>
         </is>
       </c>
     </row>
@@ -43750,27 +43750,27 @@
         </is>
       </c>
       <c r="C1291">
-        <v>4491</v>
+        <v>4421</v>
       </c>
       <c r="D1291" t="inlineStr">
         <is>
-          <t>FEC</t>
+          <t>FUNDIF</t>
         </is>
       </c>
       <c r="E1291">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F1291" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>MULTAS PECUNIARIAS E JUROS DE MORA FIXADOS EM SENTENCAS JUDICIAIS</t>
         </is>
       </c>
       <c r="G1291">
-        <v>1999992199000</v>
+        <v>1911080101000</v>
       </c>
       <c r="H1291" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
         </is>
       </c>
     </row>
@@ -43784,11 +43784,11 @@
         </is>
       </c>
       <c r="C1292">
-        <v>4331</v>
+        <v>4491</v>
       </c>
       <c r="D1292" t="inlineStr">
         <is>
-          <t>FDM</t>
+          <t>FEC</t>
         </is>
       </c>
       <c r="E1292">
@@ -43800,7 +43800,12 @@
         </is>
       </c>
       <c r="G1292">
-        <v>1739990126001</v>
+        <v>1999992199000</v>
+      </c>
+      <c r="H1292" t="inlineStr">
+        <is>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+        </is>
       </c>
     </row>
     <row r="1293">
@@ -43829,12 +43834,7 @@
         </is>
       </c>
       <c r="G1293">
-        <v>1911010199000</v>
-      </c>
-      <c r="H1293" t="inlineStr">
-        <is>
-          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - DEMAIS</t>
-        </is>
+        <v>1739990126001</v>
       </c>
     </row>
     <row r="1294">
@@ -43847,11 +43847,11 @@
         </is>
       </c>
       <c r="C1294">
-        <v>4491</v>
+        <v>4331</v>
       </c>
       <c r="D1294" t="inlineStr">
         <is>
-          <t>FEC</t>
+          <t>FDM</t>
         </is>
       </c>
       <c r="E1294">
@@ -43863,45 +43863,45 @@
         </is>
       </c>
       <c r="G1294">
-        <v>1321010101000</v>
+        <v>1911010199000</v>
       </c>
       <c r="H1294" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>MULTAS LEGISL. ESPECIFICA - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1295">
       <c r="A1295">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B1295" t="inlineStr">
         <is>
-          <t>RECURSOS DE EMOLUMENTOS, TAXAS E CUSTAS</t>
+          <t>RECURSOS VINCULADOS A FUNDOS</t>
         </is>
       </c>
       <c r="C1295">
-        <v>4031</v>
+        <v>4491</v>
       </c>
       <c r="D1295" t="inlineStr">
         <is>
-          <t>FEPJ</t>
+          <t>FEC</t>
         </is>
       </c>
       <c r="E1295">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F1295" t="inlineStr">
         <is>
-          <t>TAXA DE FISCALIZACAO JUDICIARIA E TAXAS E MULTAS JUDICIAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1295">
-        <v>1121010102000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1295" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - PRINC. - TAXA DE FISCALIZACAO JUDICIARIA</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -43931,11 +43931,11 @@
         </is>
       </c>
       <c r="G1296">
-        <v>1121010202000</v>
+        <v>1121010102000</v>
       </c>
       <c r="H1296" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - MJM - TAXA DE FISCALIZACAO JUDICIARIA</t>
+          <t>TX. INSP. CONTR. FISC. - PRINC. - TAXA DE FISCALIZACAO JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -43965,11 +43965,11 @@
         </is>
       </c>
       <c r="G1297">
-        <v>1121010302000</v>
+        <v>1121010202000</v>
       </c>
       <c r="H1297" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - DA - TAXA DE FISCALIZACAO JUDICIARIA</t>
+          <t>TX. INSP. CONTR. FISC. - MJM - TAXA DE FISCALIZACAO JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -43999,11 +43999,11 @@
         </is>
       </c>
       <c r="G1298">
-        <v>1121010402000</v>
+        <v>1121010302000</v>
       </c>
       <c r="H1298" t="inlineStr">
         <is>
-          <t>TX. INSP. CONTR. FISC. - DA-MJM - TAXA DE FISCALIZACAO JUDICIARIA</t>
+          <t>TX. INSP. CONTR. FISC. - DA - TAXA DE FISCALIZACAO JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44033,11 +44033,11 @@
         </is>
       </c>
       <c r="G1299">
-        <v>1122020101000</v>
+        <v>1121010402000</v>
       </c>
       <c r="H1299" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
+          <t>TX. INSP. CONTR. FISC. - DA-MJM - TAXA DE FISCALIZACAO JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44067,11 +44067,11 @@
         </is>
       </c>
       <c r="G1300">
-        <v>1122020102000</v>
+        <v>1122020101000</v>
       </c>
       <c r="H1300" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
         </is>
       </c>
     </row>
@@ -44101,11 +44101,11 @@
         </is>
       </c>
       <c r="G1301">
-        <v>1122020103000</v>
+        <v>1122020102000</v>
       </c>
       <c r="H1301" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - TAXA JUDICIARIA</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
         </is>
       </c>
     </row>
@@ -44135,11 +44135,11 @@
         </is>
       </c>
       <c r="G1302">
-        <v>1122020201000</v>
+        <v>1122020103000</v>
       </c>
       <c r="H1302" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - PRINC. - TAXA JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44169,11 +44169,11 @@
         </is>
       </c>
       <c r="G1303">
-        <v>1122020202000</v>
+        <v>1122020201000</v>
       </c>
       <c r="H1303" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
         </is>
       </c>
     </row>
@@ -44203,11 +44203,11 @@
         </is>
       </c>
       <c r="G1304">
-        <v>1122020203000</v>
+        <v>1122020202000</v>
       </c>
       <c r="H1304" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - TAXA JUDICIARIA</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
         </is>
       </c>
     </row>
@@ -44237,11 +44237,11 @@
         </is>
       </c>
       <c r="G1305">
-        <v>1122020301000</v>
+        <v>1122020203000</v>
       </c>
       <c r="H1305" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - MJM - TAXA JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44271,11 +44271,11 @@
         </is>
       </c>
       <c r="G1306">
-        <v>1122020302000</v>
+        <v>1122020301000</v>
       </c>
       <c r="H1306" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
         </is>
       </c>
     </row>
@@ -44305,11 +44305,11 @@
         </is>
       </c>
       <c r="G1307">
-        <v>1122020303000</v>
+        <v>1122020302000</v>
       </c>
       <c r="H1307" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - TAXA JUDICIARIA</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
         </is>
       </c>
     </row>
@@ -44339,11 +44339,11 @@
         </is>
       </c>
       <c r="G1308">
-        <v>1122020401000</v>
+        <v>1122020303000</v>
       </c>
       <c r="H1308" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA - TAXA JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44373,11 +44373,11 @@
         </is>
       </c>
       <c r="G1309">
-        <v>1122020402000</v>
+        <v>1122020401000</v>
       </c>
       <c r="H1309" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - CUSTAS JUDICIAIS - JUSTICA COMUM</t>
         </is>
       </c>
     </row>
@@ -44407,11 +44407,11 @@
         </is>
       </c>
       <c r="G1310">
-        <v>1122020403000</v>
+        <v>1122020402000</v>
       </c>
       <c r="H1310" t="inlineStr">
         <is>
-          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - TAXA JUDICIARIA</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - CUSTAS JUDICIAIS - JUIZADO ESPECIAL</t>
         </is>
       </c>
     </row>
@@ -44441,11 +44441,11 @@
         </is>
       </c>
       <c r="G1311">
-        <v>1911080101000</v>
+        <v>1122020403000</v>
       </c>
       <c r="H1311" t="inlineStr">
         <is>
-          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
+          <t>EMOLUMENTOS CUSTAS JUDICIAIS - DA-MJM - TAXA JUDICIARIA</t>
         </is>
       </c>
     </row>
@@ -44475,11 +44475,11 @@
         </is>
       </c>
       <c r="G1312">
-        <v>1911080301000</v>
+        <v>1911080101000</v>
       </c>
       <c r="H1312" t="inlineStr">
         <is>
-          <t>MULTAS SENTENCAS JUDICIAIS - DA - MULTAS PECUNIARIAS E JUROS DE MORA</t>
+          <t>MULTAS SENTENCAS JUDICIAIS - PRINC. - MULTAS PECUNIARIAS E JUROS DE MORA</t>
         </is>
       </c>
     </row>
@@ -44509,11 +44509,11 @@
         </is>
       </c>
       <c r="G1313">
-        <v>1911080401000</v>
+        <v>1911080301000</v>
       </c>
       <c r="H1313" t="inlineStr">
         <is>
-          <t>MULTAS SENTENCAS JUDICIAIS - DA-MJM - MULTAS PECUNIARIAS E JUROS DE MORA</t>
+          <t>MULTAS SENTENCAS JUDICIAIS - DA - MULTAS PECUNIARIAS E JUROS DE MORA</t>
         </is>
       </c>
     </row>
@@ -44543,11 +44543,11 @@
         </is>
       </c>
       <c r="G1314">
-        <v>1911090199000</v>
+        <v>1911080401000</v>
       </c>
       <c r="H1314" t="inlineStr">
         <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - DEMAIS</t>
+          <t>MULTAS SENTENCAS JUDICIAIS - DA-MJM - MULTAS PECUNIARIAS E JUROS DE MORA</t>
         </is>
       </c>
     </row>
@@ -44577,11 +44577,11 @@
         </is>
       </c>
       <c r="G1315">
-        <v>1921990199000</v>
+        <v>1911090199000</v>
       </c>
       <c r="H1315" t="inlineStr">
         <is>
-          <t>OUTRAS INDENIZACOES - PRINC. - DEMAIS</t>
+          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -44611,11 +44611,11 @@
         </is>
       </c>
       <c r="G1316">
-        <v>1922990199000</v>
+        <v>1921990199000</v>
       </c>
       <c r="H1316" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>OUTRAS INDENIZACOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -44645,11 +44645,11 @@
         </is>
       </c>
       <c r="G1317">
-        <v>1999992199000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1317" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -44679,45 +44679,45 @@
         </is>
       </c>
       <c r="G1318">
-        <v>1911090399000</v>
+        <v>1999992199000</v>
       </c>
       <c r="H1318" t="inlineStr">
         <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA</t>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1319">
       <c r="A1319">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B1319" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO FUNDO DE COMBATE E ERRADICAÇÃO DA POBREZA</t>
+          <t>RECURSOS DE EMOLUMENTOS, TAXAS E CUSTAS</t>
         </is>
       </c>
       <c r="C1319">
-        <v>9999</v>
+        <v>4031</v>
       </c>
       <c r="D1319" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FEPJ</t>
         </is>
       </c>
       <c r="E1319">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F1319" t="inlineStr">
         <is>
-          <t>RECURSOS DO FUNDO ESTADUAL DE ERRADICACAO DA MISERIA</t>
+          <t>TAXA DE FISCALIZACAO JUDICIARIA E TAXAS E MULTAS JUDICIAIS</t>
         </is>
       </c>
       <c r="G1319">
-        <v>1114502101000</v>
+        <v>1911090399000</v>
       </c>
       <c r="H1319" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO ESTADO</t>
+          <t>MULTAS JUROS PREVISTOS CONTRATOS - DA</t>
         </is>
       </c>
     </row>
@@ -44747,11 +44747,11 @@
         </is>
       </c>
       <c r="G1320">
-        <v>1114502201000</v>
+        <v>1114502101000</v>
       </c>
       <c r="H1320" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO ESTADO</t>
+          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO ESTADO</t>
         </is>
       </c>
     </row>
@@ -44781,11 +44781,11 @@
         </is>
       </c>
       <c r="G1321">
-        <v>1114502301000</v>
+        <v>1114502201000</v>
       </c>
       <c r="H1321" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO ESTADO</t>
+          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO ESTADO</t>
         </is>
       </c>
     </row>
@@ -44815,11 +44815,11 @@
         </is>
       </c>
       <c r="G1322">
-        <v>1114502401000</v>
+        <v>1114502301000</v>
       </c>
       <c r="H1322" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO ESTADO</t>
+          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO ESTADO</t>
         </is>
       </c>
     </row>
@@ -44849,11 +44849,11 @@
         </is>
       </c>
       <c r="G1323">
-        <v>1922990199000</v>
+        <v>1114502401000</v>
       </c>
       <c r="H1323" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO ESTADO</t>
         </is>
       </c>
     </row>
@@ -44883,45 +44883,45 @@
         </is>
       </c>
       <c r="G1324">
-        <v>1321010101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1324" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1325">
       <c r="A1325">
-        <v>799</v>
+        <v>761</v>
       </c>
       <c r="B1325" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO FUNDO DE COMBATE E ERRADICAÇÃO DA POBREZA</t>
         </is>
       </c>
       <c r="C1325">
-        <v>1231</v>
+        <v>9999</v>
       </c>
       <c r="D1325" t="inlineStr">
         <is>
-          <t>SEAPA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1325">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F1325" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS DO FUNDO ESTADUAL DE ERRADICACAO DA MISERIA</t>
         </is>
       </c>
       <c r="G1325">
-        <v>1349010103000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1325" t="inlineStr">
         <is>
-          <t>COMPENSACOES AMBIENTAIS - PRINC. - SUPRESSAO DO PEQUI</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -44935,11 +44935,11 @@
         </is>
       </c>
       <c r="C1326">
-        <v>1371</v>
+        <v>1231</v>
       </c>
       <c r="D1326" t="inlineStr">
         <is>
-          <t>SEMAD</t>
+          <t>SEAPA</t>
         </is>
       </c>
       <c r="E1326">
@@ -44951,11 +44951,11 @@
         </is>
       </c>
       <c r="G1326">
-        <v>1921990101000</v>
+        <v>1349010103000</v>
       </c>
       <c r="H1326" t="inlineStr">
         <is>
-          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
+          <t>COMPENSACOES AMBIENTAIS - PRINC. - SUPRESSAO DO PEQUI</t>
         </is>
       </c>
     </row>
@@ -44969,27 +44969,27 @@
         </is>
       </c>
       <c r="C1327">
-        <v>1911</v>
+        <v>1371</v>
       </c>
       <c r="D1327" t="inlineStr">
         <is>
-          <t>EGE - SEF</t>
+          <t>SEMAD</t>
         </is>
       </c>
       <c r="E1327">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="F1327" t="inlineStr">
         <is>
-          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1327">
-        <v>1112510102000</v>
+        <v>1921990101000</v>
       </c>
       <c r="H1327" t="inlineStr">
         <is>
-          <t>IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>
       </c>
     </row>
@@ -45019,11 +45019,11 @@
         </is>
       </c>
       <c r="G1328">
-        <v>1112510202000</v>
+        <v>1112510102000</v>
       </c>
       <c r="H1328" t="inlineStr">
         <is>
-          <t>IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45053,11 +45053,11 @@
         </is>
       </c>
       <c r="G1329">
-        <v>1112510302000</v>
+        <v>1112510202000</v>
       </c>
       <c r="H1329" t="inlineStr">
         <is>
-          <t>IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45087,11 +45087,11 @@
         </is>
       </c>
       <c r="G1330">
-        <v>1114501102000</v>
+        <v>1112510302000</v>
       </c>
       <c r="H1330" t="inlineStr">
         <is>
-          <t>ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45121,11 +45121,11 @@
         </is>
       </c>
       <c r="G1331">
-        <v>1114501202000</v>
+        <v>1114501102000</v>
       </c>
       <c r="H1331" t="inlineStr">
         <is>
-          <t>ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45155,11 +45155,11 @@
         </is>
       </c>
       <c r="G1332">
-        <v>1114501302000</v>
+        <v>1114501202000</v>
       </c>
       <c r="H1332" t="inlineStr">
         <is>
-          <t>ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45189,11 +45189,11 @@
         </is>
       </c>
       <c r="G1333">
-        <v>9112510102000</v>
+        <v>1114501302000</v>
       </c>
       <c r="H1333" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45223,11 +45223,11 @@
         </is>
       </c>
       <c r="G1334">
-        <v>9112510202000</v>
+        <v>9112510102000</v>
       </c>
       <c r="H1334" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45257,11 +45257,11 @@
         </is>
       </c>
       <c r="G1335">
-        <v>9112510302000</v>
+        <v>9112510202000</v>
       </c>
       <c r="H1335" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45291,11 +45291,11 @@
         </is>
       </c>
       <c r="G1336">
-        <v>9114501102000</v>
+        <v>9112510302000</v>
       </c>
       <c r="H1336" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45325,11 +45325,11 @@
         </is>
       </c>
       <c r="G1337">
-        <v>9114501202000</v>
+        <v>9114501102000</v>
       </c>
       <c r="H1337" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45359,11 +45359,11 @@
         </is>
       </c>
       <c r="G1338">
-        <v>9114501302000</v>
+        <v>9114501202000</v>
       </c>
       <c r="H1338" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45385,19 +45385,19 @@
         </is>
       </c>
       <c r="E1339">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1339" t="inlineStr">
         <is>
-          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
+          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
         </is>
       </c>
       <c r="G1339">
-        <v>1112510103000</v>
+        <v>9114501302000</v>
       </c>
       <c r="H1339" t="inlineStr">
         <is>
-          <t>IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -45427,11 +45427,11 @@
         </is>
       </c>
       <c r="G1340">
-        <v>1112510203000</v>
+        <v>1112510103000</v>
       </c>
       <c r="H1340" t="inlineStr">
         <is>
-          <t>IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45461,11 +45461,11 @@
         </is>
       </c>
       <c r="G1341">
-        <v>1112510303000</v>
+        <v>1112510203000</v>
       </c>
       <c r="H1341" t="inlineStr">
         <is>
-          <t>IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45495,11 +45495,11 @@
         </is>
       </c>
       <c r="G1342">
-        <v>1112520102000</v>
+        <v>1112510303000</v>
       </c>
       <c r="H1342" t="inlineStr">
         <is>
-          <t>ITCD - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45529,11 +45529,11 @@
         </is>
       </c>
       <c r="G1343">
-        <v>1112520202000</v>
+        <v>1112520102000</v>
       </c>
       <c r="H1343" t="inlineStr">
         <is>
-          <t>ITCD - MJM - COTA PARTE DO FUNDEB</t>
+          <t>ITCD - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45563,11 +45563,11 @@
         </is>
       </c>
       <c r="G1344">
-        <v>1112520302000</v>
+        <v>1112520202000</v>
       </c>
       <c r="H1344" t="inlineStr">
         <is>
-          <t>ITCD - DA - COTA PARTE DO FUNDEB</t>
+          <t>ITCD - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45597,11 +45597,11 @@
         </is>
       </c>
       <c r="G1345">
-        <v>1114501103000</v>
+        <v>1112520302000</v>
       </c>
       <c r="H1345" t="inlineStr">
         <is>
-          <t>ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ITCD - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45631,11 +45631,11 @@
         </is>
       </c>
       <c r="G1346">
-        <v>1114501203000</v>
+        <v>1114501103000</v>
       </c>
       <c r="H1346" t="inlineStr">
         <is>
-          <t>ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45665,11 +45665,11 @@
         </is>
       </c>
       <c r="G1347">
-        <v>1114501303000</v>
+        <v>1114501203000</v>
       </c>
       <c r="H1347" t="inlineStr">
         <is>
-          <t>ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45699,11 +45699,11 @@
         </is>
       </c>
       <c r="G1348">
-        <v>1114502102000</v>
+        <v>1114501303000</v>
       </c>
       <c r="H1348" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45733,11 +45733,11 @@
         </is>
       </c>
       <c r="G1349">
-        <v>1114502202000</v>
+        <v>1114502102000</v>
       </c>
       <c r="H1349" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45767,11 +45767,11 @@
         </is>
       </c>
       <c r="G1350">
-        <v>1114502302000</v>
+        <v>1114502202000</v>
       </c>
       <c r="H1350" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45801,11 +45801,11 @@
         </is>
       </c>
       <c r="G1351">
-        <v>1114502402000</v>
+        <v>1114502302000</v>
       </c>
       <c r="H1351" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45835,11 +45835,11 @@
         </is>
       </c>
       <c r="G1352">
-        <v>9112510103000</v>
+        <v>1114502402000</v>
       </c>
       <c r="H1352" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45869,11 +45869,11 @@
         </is>
       </c>
       <c r="G1353">
-        <v>9112510203000</v>
+        <v>9112510103000</v>
       </c>
       <c r="H1353" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45903,11 +45903,11 @@
         </is>
       </c>
       <c r="G1354">
-        <v>9112510303000</v>
+        <v>9112510203000</v>
       </c>
       <c r="H1354" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45937,11 +45937,11 @@
         </is>
       </c>
       <c r="G1355">
-        <v>9112520102000</v>
+        <v>9112510303000</v>
       </c>
       <c r="H1355" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -45971,11 +45971,11 @@
         </is>
       </c>
       <c r="G1356">
-        <v>9112520202000</v>
+        <v>9112520102000</v>
       </c>
       <c r="H1356" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46005,11 +46005,11 @@
         </is>
       </c>
       <c r="G1357">
-        <v>9112520302000</v>
+        <v>9112520202000</v>
       </c>
       <c r="H1357" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46039,11 +46039,11 @@
         </is>
       </c>
       <c r="G1358">
-        <v>9114501103000</v>
+        <v>9112520302000</v>
       </c>
       <c r="H1358" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46073,11 +46073,11 @@
         </is>
       </c>
       <c r="G1359">
-        <v>9114501203000</v>
+        <v>9114501103000</v>
       </c>
       <c r="H1359" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46107,11 +46107,11 @@
         </is>
       </c>
       <c r="G1360">
-        <v>9114501303000</v>
+        <v>9114501203000</v>
       </c>
       <c r="H1360" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46141,11 +46141,11 @@
         </is>
       </c>
       <c r="G1361">
-        <v>9114502102000</v>
+        <v>9114501303000</v>
       </c>
       <c r="H1361" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46175,11 +46175,11 @@
         </is>
       </c>
       <c r="G1362">
-        <v>9114502202000</v>
+        <v>9114502102000</v>
       </c>
       <c r="H1362" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46209,11 +46209,11 @@
         </is>
       </c>
       <c r="G1363">
-        <v>9114502302000</v>
+        <v>9114502202000</v>
       </c>
       <c r="H1363" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46243,11 +46243,11 @@
         </is>
       </c>
       <c r="G1364">
-        <v>9114502402000</v>
+        <v>9114502302000</v>
       </c>
       <c r="H1364" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46261,27 +46261,27 @@
         </is>
       </c>
       <c r="C1365">
-        <v>2011</v>
+        <v>1911</v>
       </c>
       <c r="D1365" t="inlineStr">
         <is>
-          <t>IPSEMG</t>
+          <t>EGE - SEF</t>
         </is>
       </c>
       <c r="E1365">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F1365" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
         </is>
       </c>
       <c r="G1365">
-        <v>1922990199000</v>
+        <v>9114502402000</v>
       </c>
       <c r="H1365" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -46311,11 +46311,11 @@
         </is>
       </c>
       <c r="G1366">
-        <v>7219991101001</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1366" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - SERVIDOR ATIVO</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -46345,11 +46345,11 @@
         </is>
       </c>
       <c r="G1367">
-        <v>7219991101002</v>
+        <v>7219991101001</v>
       </c>
       <c r="H1367" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - SERVIDOR INATIVO</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - SERVIDOR ATIVO</t>
         </is>
       </c>
     </row>
@@ -46379,11 +46379,11 @@
         </is>
       </c>
       <c r="G1368">
-        <v>7219991101003</v>
+        <v>7219991101002</v>
       </c>
       <c r="H1368" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - PENSIONISTA</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - SERVIDOR INATIVO</t>
         </is>
       </c>
     </row>
@@ -46413,11 +46413,11 @@
         </is>
       </c>
       <c r="G1369">
-        <v>7219991101004</v>
+        <v>7219991101003</v>
       </c>
       <c r="H1369" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - CONTRATO ADMINISTRATIVO</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - PENSIONISTA</t>
         </is>
       </c>
     </row>
@@ -46447,11 +46447,11 @@
         </is>
       </c>
       <c r="G1370">
-        <v>7219991101005</v>
+        <v>7219991101004</v>
       </c>
       <c r="H1370" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - ESTADO - DEPENDENTES</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - CONTRATO ADMINISTRATIVO</t>
         </is>
       </c>
     </row>
@@ -46481,11 +46481,11 @@
         </is>
       </c>
       <c r="G1371">
-        <v>7219991101006</v>
+        <v>7219991101005</v>
       </c>
       <c r="H1371" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - ESTADO - DEPENDENTES - FILHOS DE 21 A 35 ANOS</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - ESTADO - DEPENDENTES</t>
         </is>
       </c>
     </row>
@@ -46515,11 +46515,11 @@
         </is>
       </c>
       <c r="G1372">
-        <v>7219991101007</v>
+        <v>7219991101006</v>
       </c>
       <c r="H1372" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - USUARIO FACULTATIVO</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - ESTADO - DEPENDENTES - FILHOS DE 21 A 35 ANOS</t>
         </is>
       </c>
     </row>
@@ -46541,19 +46541,19 @@
         </is>
       </c>
       <c r="E1373">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1373" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1373">
-        <v>1219991102001</v>
+        <v>7219991101007</v>
       </c>
       <c r="H1373" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ATIVO</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. PATRON. CIVIL SAUDE - USUARIO FACULTATIVO</t>
         </is>
       </c>
     </row>
@@ -46583,11 +46583,11 @@
         </is>
       </c>
       <c r="G1374">
-        <v>1219991102002</v>
+        <v>1219991102001</v>
       </c>
       <c r="H1374" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - INATIVO</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ATIVO</t>
         </is>
       </c>
     </row>
@@ -46617,11 +46617,11 @@
         </is>
       </c>
       <c r="G1375">
-        <v>1219991102004</v>
+        <v>1219991102002</v>
       </c>
       <c r="H1375" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - CONTRATO ADMINISTRATIVO</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - INATIVO</t>
         </is>
       </c>
     </row>
@@ -46651,11 +46651,11 @@
         </is>
       </c>
       <c r="G1376">
-        <v>1219991102005</v>
+        <v>1219991102004</v>
       </c>
       <c r="H1376" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ESTADO - DEPENDENTES</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - CONTRATO ADMINISTRATIVO</t>
         </is>
       </c>
     </row>
@@ -46685,11 +46685,11 @@
         </is>
       </c>
       <c r="G1377">
-        <v>1219991102006</v>
+        <v>1219991102005</v>
       </c>
       <c r="H1377" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ESTADO - DEPENDENTES - FILHOS DE 21 A 35 ANOS</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ESTADO - DEPENDENTES</t>
         </is>
       </c>
     </row>
@@ -46719,11 +46719,11 @@
         </is>
       </c>
       <c r="G1378">
-        <v>1219991102007</v>
+        <v>1219991102006</v>
       </c>
       <c r="H1378" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - USUARIO FACULTATIVO</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - ESTADO - DEPENDENTES - FILHOS DE 21 A 35 ANOS</t>
         </is>
       </c>
     </row>
@@ -46753,11 +46753,11 @@
         </is>
       </c>
       <c r="G1379">
-        <v>1911090199000</v>
+        <v>1219991102007</v>
       </c>
       <c r="H1379" t="inlineStr">
         <is>
-          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - DEMAIS</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - CONTRIB. CIVIL SAUDE - USUARIO FACULTATIVO</t>
         </is>
       </c>
     </row>
@@ -46787,11 +46787,11 @@
         </is>
       </c>
       <c r="G1380">
-        <v>1922990199000</v>
+        <v>1911090199000</v>
       </c>
       <c r="H1380" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>MULTAS JUROS PREVISTOS CONTRATOS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -46805,27 +46805,27 @@
         </is>
       </c>
       <c r="C1381">
-        <v>2101</v>
+        <v>2011</v>
       </c>
       <c r="D1381" t="inlineStr">
         <is>
-          <t>IEF</t>
+          <t>IPSEMG</t>
         </is>
       </c>
       <c r="E1381">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F1381" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1381">
-        <v>1349010101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1381" t="inlineStr">
         <is>
-          <t>COMPENSACOES AMBIENTAIS - PRINC. - REPOSICAO FLORESTAL</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -46855,11 +46855,11 @@
         </is>
       </c>
       <c r="G1382">
-        <v>1349010102000</v>
+        <v>1349010101000</v>
       </c>
       <c r="H1382" t="inlineStr">
         <is>
-          <t>COMPENSACOES AMBIENTAIS - PRINC. - REPOSICAO DA PESCA</t>
+          <t>COMPENSACOES AMBIENTAIS - PRINC. - REPOSICAO FLORESTAL</t>
         </is>
       </c>
     </row>
@@ -46889,11 +46889,11 @@
         </is>
       </c>
       <c r="G1383">
-        <v>1349010199000</v>
+        <v>1349010102000</v>
       </c>
       <c r="H1383" t="inlineStr">
         <is>
-          <t>COMPENSACOES AMBIENTAIS - PRINC. - DEMAIS</t>
+          <t>COMPENSACOES AMBIENTAIS - PRINC. - REPOSICAO DA PESCA</t>
         </is>
       </c>
     </row>
@@ -46923,11 +46923,11 @@
         </is>
       </c>
       <c r="G1384">
-        <v>1611010118000</v>
+        <v>1349010199000</v>
       </c>
       <c r="H1384" t="inlineStr">
         <is>
-          <t>SERVICOS ADM. COMERC. GER. - PRINC. - VISITACAO DAS UNIDADES DE CONSERVACAO DA NATUREZA</t>
+          <t>COMPENSACOES AMBIENTAIS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -46957,11 +46957,11 @@
         </is>
       </c>
       <c r="G1385">
-        <v>1922990199000</v>
+        <v>1611010118000</v>
       </c>
       <c r="H1385" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>SERVICOS ADM. COMERC. GER. - PRINC. - VISITACAO DAS UNIDADES DE CONSERVACAO DA NATUREZA</t>
         </is>
       </c>
     </row>
@@ -46975,27 +46975,27 @@
         </is>
       </c>
       <c r="C1386">
-        <v>2121</v>
+        <v>2101</v>
       </c>
       <c r="D1386" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>IEF</t>
         </is>
       </c>
       <c r="E1386">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F1386" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1386">
-        <v>7215532101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1386" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - SAUDE</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47025,11 +47025,11 @@
         </is>
       </c>
       <c r="G1387">
-        <v>7219991103051</v>
+        <v>7215532101000</v>
       </c>
       <c r="H1387" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - ATIVO CIVIL</t>
+          <t>REC. INTRA. - CONTRIB. PATRONAL MILITAR INATIVO - PRINC. - SAUDE</t>
         </is>
       </c>
     </row>
@@ -47051,19 +47051,19 @@
         </is>
       </c>
       <c r="E1388">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1388" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1388">
-        <v>1215521103000</v>
+        <v>7219991103051</v>
       </c>
       <c r="H1388" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SAUDE</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - ATIVO CIVIL</t>
         </is>
       </c>
     </row>
@@ -47093,11 +47093,11 @@
         </is>
       </c>
       <c r="G1389">
-        <v>1219991103001</v>
+        <v>1215521103000</v>
       </c>
       <c r="H1389" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. DO SERVIDOR CIVIL - ATIVO</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SAUDE</t>
         </is>
       </c>
     </row>
@@ -47127,11 +47127,11 @@
         </is>
       </c>
       <c r="G1390">
-        <v>1219991103002</v>
+        <v>1219991103001</v>
       </c>
       <c r="H1390" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. DO SERVIDOR CIVIL - INATIVO</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. DO SERVIDOR CIVIL - ATIVO</t>
         </is>
       </c>
     </row>
@@ -47161,11 +47161,11 @@
         </is>
       </c>
       <c r="G1391">
-        <v>7219991103051</v>
+        <v>1219991103002</v>
       </c>
       <c r="H1391" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - ATIVO CIVIL</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. DO SERVIDOR CIVIL - INATIVO</t>
         </is>
       </c>
     </row>
@@ -47179,27 +47179,27 @@
         </is>
       </c>
       <c r="C1392">
-        <v>2241</v>
+        <v>2121</v>
       </c>
       <c r="D1392" t="inlineStr">
         <is>
-          <t>IGAM</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1392">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F1392" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1392">
-        <v>1345010101000</v>
+        <v>7219991103051</v>
       </c>
       <c r="H1392" t="inlineStr">
         <is>
-          <t>OUTORGA DIR. USO RECURSOS HIDRICOS - PRINC.</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - ATIVO CIVIL</t>
         </is>
       </c>
     </row>
@@ -47229,11 +47229,11 @@
         </is>
       </c>
       <c r="G1393">
-        <v>1345010301000</v>
+        <v>1345010101000</v>
       </c>
       <c r="H1393" t="inlineStr">
         <is>
-          <t>OUTORGA DIR. USO RECURSOS HIDRICOS - DA</t>
+          <t>OUTORGA DIR. USO RECURSOS HIDRICOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -47247,27 +47247,27 @@
         </is>
       </c>
       <c r="C1394">
-        <v>2361</v>
+        <v>2241</v>
       </c>
       <c r="D1394" t="inlineStr">
         <is>
-          <t>IPLEMG</t>
+          <t>IGAM</t>
         </is>
       </c>
       <c r="E1394">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1394" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1394">
-        <v>1219991104001</v>
+        <v>1345010301000</v>
       </c>
       <c r="H1394" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - ATIVO - EXERCENTE DE MANDATO ELETIVO E OUTROS CIVIS</t>
+          <t>OUTORGA DIR. USO RECURSOS HIDRICOS - DA</t>
         </is>
       </c>
     </row>
@@ -47297,11 +47297,11 @@
         </is>
       </c>
       <c r="G1395">
-        <v>1219991104002</v>
+        <v>1219991104001</v>
       </c>
       <c r="H1395" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - INATIVO</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - ATIVO - EXERCENTE DE MANDATO ELETIVO E OUTROS CIVIS</t>
         </is>
       </c>
     </row>
@@ -47331,11 +47331,11 @@
         </is>
       </c>
       <c r="G1396">
-        <v>1219991104003</v>
+        <v>1219991104002</v>
       </c>
       <c r="H1396" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - PENSIONISTA</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - INATIVO</t>
         </is>
       </c>
     </row>
@@ -47365,11 +47365,11 @@
         </is>
       </c>
       <c r="G1397">
-        <v>1219991104052</v>
+        <v>1219991104003</v>
       </c>
       <c r="H1397" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. PATRONAL - EXERCENTE DE MANDATO ELETIVO FEDERAL OU MUNICIPAL</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. DO SEGURADO - PENSIONISTA</t>
         </is>
       </c>
     </row>
@@ -47399,11 +47399,11 @@
         </is>
       </c>
       <c r="G1398">
-        <v>1311011101000</v>
+        <v>1219991104052</v>
       </c>
       <c r="H1398" t="inlineStr">
         <is>
-          <t>ALUGUEIS ARRENDAMENTOS - PRINC. - ALUGUEIS</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. PATRONAL - EXERCENTE DE MANDATO ELETIVO FEDERAL OU MUNICIPAL</t>
         </is>
       </c>
     </row>
@@ -47433,11 +47433,11 @@
         </is>
       </c>
       <c r="G1399">
-        <v>1321040101000</v>
+        <v>1311011101000</v>
       </c>
       <c r="H1399" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
+          <t>ALUGUEIS ARRENDAMENTOS - PRINC. - ALUGUEIS</t>
         </is>
       </c>
     </row>
@@ -47467,11 +47467,11 @@
         </is>
       </c>
       <c r="G1400">
-        <v>1321040102000</v>
+        <v>1321040101000</v>
       </c>
       <c r="H1400" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
         </is>
       </c>
     </row>
@@ -47501,11 +47501,11 @@
         </is>
       </c>
       <c r="G1401">
-        <v>1322010102000</v>
+        <v>1321040102000</v>
       </c>
       <c r="H1401" t="inlineStr">
         <is>
-          <t>DIVIDENDOS - PRINC. - EMPRESAS NAO ESTATAIS</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
         </is>
       </c>
     </row>
@@ -47535,11 +47535,11 @@
         </is>
       </c>
       <c r="G1402">
-        <v>1641010101000</v>
+        <v>1322010102000</v>
       </c>
       <c r="H1402" t="inlineStr">
         <is>
-          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
+          <t>DIVIDENDOS - PRINC. - EMPRESAS NAO ESTATAIS</t>
         </is>
       </c>
     </row>
@@ -47569,11 +47569,11 @@
         </is>
       </c>
       <c r="G1403">
-        <v>1641010199000</v>
+        <v>1641010101000</v>
       </c>
       <c r="H1403" t="inlineStr">
         <is>
-          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - DEMAIS</t>
+          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
         </is>
       </c>
     </row>
@@ -47603,11 +47603,11 @@
         </is>
       </c>
       <c r="G1404">
-        <v>1922990199000</v>
+        <v>1641010199000</v>
       </c>
       <c r="H1404" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47637,11 +47637,11 @@
         </is>
       </c>
       <c r="G1405">
-        <v>1999992199000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1405" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47671,11 +47671,11 @@
         </is>
       </c>
       <c r="G1406">
-        <v>2999990101000</v>
+        <v>1999992199000</v>
       </c>
       <c r="H1406" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - RESERVA ATUARIAL</t>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47705,11 +47705,11 @@
         </is>
       </c>
       <c r="G1407">
-        <v>2999990199000</v>
+        <v>2999990101000</v>
       </c>
       <c r="H1407" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - DEMAIS</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - RESERVA ATUARIAL</t>
         </is>
       </c>
     </row>
@@ -47739,11 +47739,11 @@
         </is>
       </c>
       <c r="G1408">
-        <v>7219991104051</v>
+        <v>2999990199000</v>
       </c>
       <c r="H1408" t="inlineStr">
         <is>
-          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. PATRONAL - EXERCENTE DE MANDATO ESTADUAL</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47773,11 +47773,11 @@
         </is>
       </c>
       <c r="G1409">
-        <v>7999992105000</v>
+        <v>7219991104051</v>
       </c>
       <c r="H1409" t="inlineStr">
         <is>
-          <t>REC. INTRA. - OUTRAS REC. - PRIMARIAS - PRINC. - RESERVA TECNICA OBRIGATORIA - EQUILIBRIO ATUARIAL</t>
+          <t>REC. INTRA. - DEMAIS CONTRIB. SOC. - PRINC. - IPLEMG - CONTRIB. PATRONAL - EXERCENTE DE MANDATO ESTADUAL</t>
         </is>
       </c>
     </row>
@@ -47791,27 +47791,27 @@
         </is>
       </c>
       <c r="C1410">
-        <v>4111</v>
+        <v>2361</v>
       </c>
       <c r="D1410" t="inlineStr">
         <is>
-          <t>FUNDESE</t>
+          <t>IPLEMG</t>
         </is>
       </c>
       <c r="E1410">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1410" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS</t>
         </is>
       </c>
       <c r="G1410">
-        <v>1641010101000</v>
+        <v>7999992105000</v>
       </c>
       <c r="H1410" t="inlineStr">
         <is>
-          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
+          <t>REC. INTRA. - OUTRAS REC. - PRIMARIAS - PRINC. - RESERVA TECNICA OBRIGATORIA - EQUILIBRIO ATUARIAL</t>
         </is>
       </c>
     </row>
@@ -47841,11 +47841,11 @@
         </is>
       </c>
       <c r="G1411">
-        <v>2311071199000</v>
+        <v>1641010101000</v>
       </c>
       <c r="H1411" t="inlineStr">
         <is>
-          <t>AMORTIZACAO FINANCIAMENTOS GERAL - PRINC. - DEMAIS</t>
+          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
         </is>
       </c>
     </row>
@@ -47859,27 +47859,27 @@
         </is>
       </c>
       <c r="C1412">
-        <v>9999</v>
+        <v>4111</v>
       </c>
       <c r="D1412" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FUNDESE</t>
         </is>
       </c>
       <c r="E1412">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F1412" t="inlineStr">
         <is>
-          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1412">
-        <v>1112510102000</v>
+        <v>2311071199000</v>
       </c>
       <c r="H1412" t="inlineStr">
         <is>
-          <t>IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>AMORTIZACAO FINANCIAMENTOS GERAL - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -47909,11 +47909,11 @@
         </is>
       </c>
       <c r="G1413">
-        <v>1112510202000</v>
+        <v>1112510102000</v>
       </c>
       <c r="H1413" t="inlineStr">
         <is>
-          <t>IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -47943,11 +47943,11 @@
         </is>
       </c>
       <c r="G1414">
-        <v>1112510302000</v>
+        <v>1112510202000</v>
       </c>
       <c r="H1414" t="inlineStr">
         <is>
-          <t>IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -47977,11 +47977,11 @@
         </is>
       </c>
       <c r="G1415">
-        <v>1114501102000</v>
+        <v>1112510302000</v>
       </c>
       <c r="H1415" t="inlineStr">
         <is>
-          <t>ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48011,11 +48011,11 @@
         </is>
       </c>
       <c r="G1416">
-        <v>1114501202000</v>
+        <v>1114501102000</v>
       </c>
       <c r="H1416" t="inlineStr">
         <is>
-          <t>ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48045,11 +48045,11 @@
         </is>
       </c>
       <c r="G1417">
-        <v>1114501302000</v>
+        <v>1114501202000</v>
       </c>
       <c r="H1417" t="inlineStr">
         <is>
-          <t>ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48079,11 +48079,11 @@
         </is>
       </c>
       <c r="G1418">
-        <v>1711530102000</v>
+        <v>1114501302000</v>
       </c>
       <c r="H1418" t="inlineStr">
         <is>
-          <t>COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - MUNICIPIOS</t>
+          <t>ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48113,11 +48113,11 @@
         </is>
       </c>
       <c r="G1419">
-        <v>9112510102000</v>
+        <v>1711530102000</v>
       </c>
       <c r="H1419" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48147,11 +48147,11 @@
         </is>
       </c>
       <c r="G1420">
-        <v>9112510202000</v>
+        <v>9112510102000</v>
       </c>
       <c r="H1420" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48181,11 +48181,11 @@
         </is>
       </c>
       <c r="G1421">
-        <v>9112510302000</v>
+        <v>9112510202000</v>
       </c>
       <c r="H1421" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48215,11 +48215,11 @@
         </is>
       </c>
       <c r="G1422">
-        <v>9114501102000</v>
+        <v>9112510302000</v>
       </c>
       <c r="H1422" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48249,11 +48249,11 @@
         </is>
       </c>
       <c r="G1423">
-        <v>9114501202000</v>
+        <v>9114501102000</v>
       </c>
       <c r="H1423" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48283,11 +48283,11 @@
         </is>
       </c>
       <c r="G1424">
-        <v>9114501302000</v>
+        <v>9114501202000</v>
       </c>
       <c r="H1424" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
+          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48317,11 +48317,11 @@
         </is>
       </c>
       <c r="G1425">
-        <v>9711530102000</v>
+        <v>9114501302000</v>
       </c>
       <c r="H1425" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - MUNICIPIOS</t>
+          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48343,19 +48343,19 @@
         </is>
       </c>
       <c r="E1426">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1426" t="inlineStr">
         <is>
-          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
+          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
         </is>
       </c>
       <c r="G1426">
-        <v>1112510103000</v>
+        <v>9711530102000</v>
       </c>
       <c r="H1426" t="inlineStr">
         <is>
-          <t>IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -48385,11 +48385,11 @@
         </is>
       </c>
       <c r="G1427">
-        <v>1112510203000</v>
+        <v>1112510103000</v>
       </c>
       <c r="H1427" t="inlineStr">
         <is>
-          <t>IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48419,11 +48419,11 @@
         </is>
       </c>
       <c r="G1428">
-        <v>1112510303000</v>
+        <v>1112510203000</v>
       </c>
       <c r="H1428" t="inlineStr">
         <is>
-          <t>IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48453,11 +48453,11 @@
         </is>
       </c>
       <c r="G1429">
-        <v>1112520102000</v>
+        <v>1112510303000</v>
       </c>
       <c r="H1429" t="inlineStr">
         <is>
-          <t>ITCD - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48487,11 +48487,11 @@
         </is>
       </c>
       <c r="G1430">
-        <v>1112520202000</v>
+        <v>1112520102000</v>
       </c>
       <c r="H1430" t="inlineStr">
         <is>
-          <t>ITCD - MJM - COTA PARTE DO FUNDEB</t>
+          <t>ITCD - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48521,11 +48521,11 @@
         </is>
       </c>
       <c r="G1431">
-        <v>1112520302000</v>
+        <v>1112520202000</v>
       </c>
       <c r="H1431" t="inlineStr">
         <is>
-          <t>ITCD - DA - COTA PARTE DO FUNDEB</t>
+          <t>ITCD - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48555,11 +48555,11 @@
         </is>
       </c>
       <c r="G1432">
-        <v>1114501103000</v>
+        <v>1112520302000</v>
       </c>
       <c r="H1432" t="inlineStr">
         <is>
-          <t>ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ITCD - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48589,11 +48589,11 @@
         </is>
       </c>
       <c r="G1433">
-        <v>1114501203000</v>
+        <v>1114501103000</v>
       </c>
       <c r="H1433" t="inlineStr">
         <is>
-          <t>ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48623,11 +48623,11 @@
         </is>
       </c>
       <c r="G1434">
-        <v>1114501303000</v>
+        <v>1114501203000</v>
       </c>
       <c r="H1434" t="inlineStr">
         <is>
-          <t>ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48657,11 +48657,11 @@
         </is>
       </c>
       <c r="G1435">
-        <v>1114502102000</v>
+        <v>1114501303000</v>
       </c>
       <c r="H1435" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48691,11 +48691,11 @@
         </is>
       </c>
       <c r="G1436">
-        <v>1114502202000</v>
+        <v>1114502102000</v>
       </c>
       <c r="H1436" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48725,11 +48725,11 @@
         </is>
       </c>
       <c r="G1437">
-        <v>1114502302000</v>
+        <v>1114502202000</v>
       </c>
       <c r="H1437" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48759,11 +48759,11 @@
         </is>
       </c>
       <c r="G1438">
-        <v>1114502402000</v>
+        <v>1114502302000</v>
       </c>
       <c r="H1438" t="inlineStr">
         <is>
-          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48793,11 +48793,11 @@
         </is>
       </c>
       <c r="G1439">
-        <v>1711500102000</v>
+        <v>1114502402000</v>
       </c>
       <c r="H1439" t="inlineStr">
         <is>
-          <t>COTA-PARTE FPE - PRINC. - FUNDEB</t>
+          <t>ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48827,11 +48827,11 @@
         </is>
       </c>
       <c r="G1440">
-        <v>1711530103000</v>
+        <v>1711500102000</v>
       </c>
       <c r="H1440" t="inlineStr">
         <is>
-          <t>COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - FUNDEB</t>
+          <t>COTA-PARTE FPE - PRINC. - FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48861,11 +48861,11 @@
         </is>
       </c>
       <c r="G1441">
-        <v>9112510103000</v>
+        <v>1711530103000</v>
       </c>
       <c r="H1441" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48895,11 +48895,11 @@
         </is>
       </c>
       <c r="G1442">
-        <v>9112510203000</v>
+        <v>9112510103000</v>
       </c>
       <c r="H1442" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48929,11 +48929,11 @@
         </is>
       </c>
       <c r="G1443">
-        <v>9112510303000</v>
+        <v>9112510203000</v>
       </c>
       <c r="H1443" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48963,11 +48963,11 @@
         </is>
       </c>
       <c r="G1444">
-        <v>9112520102000</v>
+        <v>9112510303000</v>
       </c>
       <c r="H1444" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - IPVA - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -48997,11 +48997,11 @@
         </is>
       </c>
       <c r="G1445">
-        <v>9112520202000</v>
+        <v>9112520102000</v>
       </c>
       <c r="H1445" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49031,11 +49031,11 @@
         </is>
       </c>
       <c r="G1446">
-        <v>9112520302000</v>
+        <v>9112520202000</v>
       </c>
       <c r="H1446" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ITCD - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49065,11 +49065,11 @@
         </is>
       </c>
       <c r="G1447">
-        <v>9114501103000</v>
+        <v>9112520302000</v>
       </c>
       <c r="H1447" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ITCD - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49099,11 +49099,11 @@
         </is>
       </c>
       <c r="G1448">
-        <v>9114501203000</v>
+        <v>9114501103000</v>
       </c>
       <c r="H1448" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - PRINC. - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49133,11 +49133,11 @@
         </is>
       </c>
       <c r="G1449">
-        <v>9114501303000</v>
+        <v>9114501203000</v>
       </c>
       <c r="H1449" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - MJM - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49167,11 +49167,11 @@
         </is>
       </c>
       <c r="G1450">
-        <v>9114502102000</v>
+        <v>9114501303000</v>
       </c>
       <c r="H1450" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ICMS - DA - COTA PARTE DO ESTADO PARA O FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49201,11 +49201,11 @@
         </is>
       </c>
       <c r="G1451">
-        <v>9114502202000</v>
+        <v>9114502102000</v>
       </c>
       <c r="H1451" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49235,11 +49235,11 @@
         </is>
       </c>
       <c r="G1452">
-        <v>9114502302000</v>
+        <v>9114502202000</v>
       </c>
       <c r="H1452" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49269,11 +49269,11 @@
         </is>
       </c>
       <c r="G1453">
-        <v>9114502402000</v>
+        <v>9114502302000</v>
       </c>
       <c r="H1453" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49303,11 +49303,11 @@
         </is>
       </c>
       <c r="G1454">
-        <v>9711500102000</v>
+        <v>9114502402000</v>
       </c>
       <c r="H1454" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - COTA-PARTE FPE - PRINC. - FUNDEB</t>
+          <t>DEDUCAO REC. - ADICIONAL ICMS - FEM - DA-MJM - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49337,11 +49337,11 @@
         </is>
       </c>
       <c r="G1455">
-        <v>9711530103000</v>
+        <v>9711500102000</v>
       </c>
       <c r="H1455" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - FUNDEB</t>
+          <t>DEDUCAO REC. - COTA-PARTE FPE - PRINC. - FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49363,19 +49363,19 @@
         </is>
       </c>
       <c r="E1456">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F1456" t="inlineStr">
         <is>
-          <t>RECURSOS FUNDOS EXTINTOS-LEI NO 13.848/2001</t>
+          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
         </is>
       </c>
       <c r="G1456">
-        <v>1641010101000</v>
+        <v>9711530103000</v>
       </c>
       <c r="H1456" t="inlineStr">
         <is>
-          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
+          <t>DEDUCAO REC. - COTA-PARTE IPI - ESTADOS EXPORT. PROD. INDUST. - PRINC. - FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49405,11 +49405,11 @@
         </is>
       </c>
       <c r="G1457">
-        <v>2311071199000</v>
+        <v>1641010101000</v>
       </c>
       <c r="H1457" t="inlineStr">
         <is>
-          <t>AMORTIZACAO FINANCIAMENTOS GERAL - PRINC. - DEMAIS</t>
+          <t>RETORNO OPER. JUROS ENCARG. FINANCEIROS - PRINC. - JUROS DE EMPRESTIMOS</t>
         </is>
       </c>
     </row>
@@ -49431,19 +49431,19 @@
         </is>
       </c>
       <c r="E1458">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="F1458" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS FUNDOS EXTINTOS-LEI NO 13.848/2001</t>
         </is>
       </c>
       <c r="G1458">
-        <v>1332040101000</v>
+        <v>2311071199000</v>
       </c>
       <c r="H1458" t="inlineStr">
         <is>
-          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+          <t>AMORTIZACAO FINANCIAMENTOS GERAL - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -49473,11 +49473,11 @@
         </is>
       </c>
       <c r="G1459">
-        <v>1349010103000</v>
+        <v>1332040101000</v>
       </c>
       <c r="H1459" t="inlineStr">
         <is>
-          <t>COMPENSACOES AMBIENTAIS - PRINC. - SUPRESSAO DO PEQUI</t>
+          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
         </is>
       </c>
     </row>
@@ -49507,11 +49507,11 @@
         </is>
       </c>
       <c r="G1460">
-        <v>1921990101000</v>
+        <v>1349010103000</v>
       </c>
       <c r="H1460" t="inlineStr">
         <is>
-          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
+          <t>COMPENSACOES AMBIENTAIS - PRINC. - SUPRESSAO DO PEQUI</t>
         </is>
       </c>
     </row>
@@ -49533,19 +49533,19 @@
         </is>
       </c>
       <c r="E1461">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1461" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1461">
-        <v>1411010102001</v>
+        <v>1921990101000</v>
       </c>
       <c r="H1461" t="inlineStr">
         <is>
-          <t>REC. AGROPECUARIA - PRINC. - PRODUCAO ANIMAL DERIVADOS - UNIDADES PENAIS</t>
+          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>
       </c>
     </row>
@@ -49575,11 +49575,11 @@
         </is>
       </c>
       <c r="G1462">
-        <v>1511010101005</v>
+        <v>1411010102001</v>
       </c>
       <c r="H1462" t="inlineStr">
         <is>
-          <t>REC. INDUSTRIAL - PRINC. - INDUSTRIA TRANSFORMACAO - INDUSTRIAS DIVERSAS - UNIDADES PENAIS</t>
+          <t>REC. AGROPECUARIA - PRINC. - PRODUCAO ANIMAL DERIVADOS - UNIDADES PENAIS</t>
         </is>
       </c>
     </row>
@@ -49593,11 +49593,11 @@
         </is>
       </c>
       <c r="C1463">
-        <v>1451</v>
+        <v>9999</v>
       </c>
       <c r="D1463" t="inlineStr">
         <is>
-          <t>SEJUSP</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1463">
@@ -49627,27 +49627,27 @@
         </is>
       </c>
       <c r="C1464">
-        <v>2121</v>
+        <v>1451</v>
       </c>
       <c r="D1464" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>SEJUSP</t>
         </is>
       </c>
       <c r="E1464">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F1464" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1464">
-        <v>7215531101000</v>
+        <v>1511010101005</v>
       </c>
       <c r="H1464" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - SAUDE</t>
+          <t>REC. INDUSTRIAL - PRINC. - INDUSTRIA TRANSFORMACAO - INDUSTRIAS DIVERSAS - UNIDADES PENAIS</t>
         </is>
       </c>
     </row>
@@ -49661,27 +49661,27 @@
         </is>
       </c>
       <c r="C1465">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1465" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1465">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="F1465" t="inlineStr">
         <is>
-          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1465">
-        <v>1719620102000</v>
+        <v>7215531101000</v>
       </c>
       <c r="H1465" t="inlineStr">
         <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - MILITAR ATIVO - PRINC. - SAUDE</t>
         </is>
       </c>
     </row>
@@ -49711,11 +49711,11 @@
         </is>
       </c>
       <c r="G1466">
-        <v>9719620102000</v>
+        <v>1719620102000</v>
       </c>
       <c r="H1466" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N? 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
+          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -49737,19 +49737,19 @@
         </is>
       </c>
       <c r="E1467">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1467" t="inlineStr">
         <is>
-          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
+          <t>RECURSOS CONSTITUC.VINCULADOS AOS MUNICIPIOS</t>
         </is>
       </c>
       <c r="G1467">
-        <v>1719620103000</v>
+        <v>9719620102000</v>
       </c>
       <c r="H1467" t="inlineStr">
         <is>
-          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N? 194/2022 - PRINC. - COTA PARTE DOS MUNICIPIOS</t>
         </is>
       </c>
     </row>
@@ -49779,11 +49779,11 @@
         </is>
       </c>
       <c r="G1468">
-        <v>9719620103000</v>
+        <v>1719620103000</v>
       </c>
       <c r="H1468" t="inlineStr">
         <is>
-          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N? 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
+          <t>TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49805,19 +49805,19 @@
         </is>
       </c>
       <c r="E1469">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="F1469" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>FUNDO DE MANUTENCAO E DESENVOLVIMENTO DA EDUCACAO BASICA - FUNDEB</t>
         </is>
       </c>
       <c r="G1469">
-        <v>1321010101000</v>
+        <v>9719620103000</v>
       </c>
       <c r="H1469" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>DEDUCAO REC. - TRANSF. COMPENS. FINANC. PERDAS ARRECAD. ICMS - LC N? 194/2022 - PRINC. - COTA PARTE DO FUNDEB</t>
         </is>
       </c>
     </row>
@@ -49831,27 +49831,27 @@
         </is>
       </c>
       <c r="C1470">
-        <v>2121</v>
+        <v>9999</v>
       </c>
       <c r="D1470" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1470">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F1470" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1470">
-        <v>1219991103052</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1470" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - INATIVO CIVIL</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -49873,19 +49873,19 @@
         </is>
       </c>
       <c r="E1471">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1471" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1471">
-        <v>1215522103000</v>
+        <v>1219991103052</v>
       </c>
       <c r="H1471" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SAUDE</t>
+          <t>DEMAIS CONTRIB. SOC. - PRINC. - IPSM - CONTRIB. PATRONAL - INATIVO CIVIL</t>
         </is>
       </c>
     </row>
@@ -49899,23 +49899,28 @@
         </is>
       </c>
       <c r="C1472">
-        <v>2101</v>
+        <v>2121</v>
       </c>
       <c r="D1472" t="inlineStr">
         <is>
-          <t>IEF</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1472">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F1472" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1472">
-        <v>1349010301000</v>
+        <v>1215522103000</v>
+      </c>
+      <c r="H1472" t="inlineStr">
+        <is>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SAUDE</t>
+        </is>
       </c>
     </row>
     <row r="1473">
@@ -49944,7 +49949,7 @@
         </is>
       </c>
       <c r="G1473">
-        <v>1349010401000</v>
+        <v>1349010301000</v>
       </c>
     </row>
     <row r="1474">
@@ -49957,23 +49962,23 @@
         </is>
       </c>
       <c r="C1474">
-        <v>9999</v>
+        <v>2101</v>
       </c>
       <c r="D1474" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IEF</t>
         </is>
       </c>
       <c r="E1474">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1474" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1474">
-        <v>1741990140001</v>
+        <v>1349010401000</v>
       </c>
     </row>
     <row r="1475">
@@ -49986,28 +49991,23 @@
         </is>
       </c>
       <c r="C1475">
-        <v>2241</v>
+        <v>9999</v>
       </c>
       <c r="D1475" t="inlineStr">
         <is>
-          <t>IGAM</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1475">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1475" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1475">
-        <v>1922990199000</v>
-      </c>
-      <c r="H1475" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
-        </is>
+        <v>1741990140001</v>
       </c>
     </row>
     <row r="1476">
@@ -50020,27 +50020,27 @@
         </is>
       </c>
       <c r="C1476">
-        <v>2091</v>
+        <v>2241</v>
       </c>
       <c r="D1476" t="inlineStr">
         <is>
-          <t>FEAM</t>
+          <t>IGAM</t>
         </is>
       </c>
       <c r="E1476">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1476" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1476">
-        <v>1921990101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1476" t="inlineStr">
         <is>
-          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -50054,27 +50054,27 @@
         </is>
       </c>
       <c r="C1477">
-        <v>2361</v>
+        <v>2091</v>
       </c>
       <c r="D1477" t="inlineStr">
         <is>
-          <t>IPLEMG</t>
+          <t>FEAM</t>
         </is>
       </c>
       <c r="E1477">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1477" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1477">
-        <v>1321010101000</v>
+        <v>1921990101000</v>
       </c>
       <c r="H1477" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>
       </c>
     </row>
@@ -50088,27 +50088,27 @@
         </is>
       </c>
       <c r="C1478">
-        <v>9999</v>
+        <v>2361</v>
       </c>
       <c r="D1478" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPLEMG</t>
         </is>
       </c>
       <c r="E1478">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F1478" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS</t>
         </is>
       </c>
       <c r="G1478">
-        <v>1741990141999</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1478" t="inlineStr">
         <is>
-          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -50138,41 +50138,41 @@
         </is>
       </c>
       <c r="G1479">
-        <v>1911090101006</v>
+        <v>1741990141999</v>
+      </c>
+      <c r="H1479" t="inlineStr">
+        <is>
+          <t>DIREITOS HUMANOS E DE CIDADANIA - OUTROS</t>
+        </is>
       </c>
     </row>
     <row r="1480">
       <c r="A1480">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1480" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1480">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1480" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1480">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F1480" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1480">
-        <v>7215021101001</v>
-      </c>
-      <c r="H1480" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>1911090101006</v>
       </c>
     </row>
     <row r="1481">
@@ -50201,11 +50201,11 @@
         </is>
       </c>
       <c r="G1481">
-        <v>7215021101002</v>
+        <v>7215021101001</v>
       </c>
       <c r="H1481" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50235,11 +50235,11 @@
         </is>
       </c>
       <c r="G1482">
-        <v>7215021102001</v>
+        <v>7215021101002</v>
       </c>
       <c r="H1482" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
         </is>
       </c>
     </row>
@@ -50269,11 +50269,11 @@
         </is>
       </c>
       <c r="G1483">
-        <v>7215021103001</v>
+        <v>7215021102001</v>
       </c>
       <c r="H1483" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50303,11 +50303,11 @@
         </is>
       </c>
       <c r="G1484">
-        <v>7215021104001</v>
+        <v>7215021103001</v>
       </c>
       <c r="H1484" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50337,11 +50337,11 @@
         </is>
       </c>
       <c r="G1485">
-        <v>7215021105001</v>
+        <v>7215021104001</v>
       </c>
       <c r="H1485" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50371,11 +50371,11 @@
         </is>
       </c>
       <c r="G1486">
-        <v>7215021106001</v>
+        <v>7215021105001</v>
       </c>
       <c r="H1486" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50405,11 +50405,11 @@
         </is>
       </c>
       <c r="G1487">
-        <v>7215021107001</v>
+        <v>7215021106001</v>
       </c>
       <c r="H1487" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50431,19 +50431,19 @@
         </is>
       </c>
       <c r="E1488">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1488" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1488">
-        <v>1215011101000</v>
+        <v>7215021107001</v>
       </c>
       <c r="H1488" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -50473,11 +50473,11 @@
         </is>
       </c>
       <c r="G1489">
-        <v>1215011102000</v>
+        <v>1215011101000</v>
       </c>
       <c r="H1489" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -50507,11 +50507,11 @@
         </is>
       </c>
       <c r="G1490">
-        <v>1215011103000</v>
+        <v>1215011102000</v>
       </c>
       <c r="H1490" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -50541,11 +50541,11 @@
         </is>
       </c>
       <c r="G1491">
-        <v>1215011104000</v>
+        <v>1215011103000</v>
       </c>
       <c r="H1491" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -50575,11 +50575,11 @@
         </is>
       </c>
       <c r="G1492">
-        <v>1215011105000</v>
+        <v>1215011104000</v>
       </c>
       <c r="H1492" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -50609,11 +50609,11 @@
         </is>
       </c>
       <c r="G1493">
-        <v>1215011106000</v>
+        <v>1215011105000</v>
       </c>
       <c r="H1493" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -50643,11 +50643,11 @@
         </is>
       </c>
       <c r="G1494">
-        <v>1215011107000</v>
+        <v>1215011106000</v>
       </c>
       <c r="H1494" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -50677,11 +50677,11 @@
         </is>
       </c>
       <c r="G1495">
-        <v>1215011199001</v>
+        <v>1215011107000</v>
       </c>
       <c r="H1495" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -50711,11 +50711,11 @@
         </is>
       </c>
       <c r="G1496">
-        <v>1215012101000</v>
+        <v>1215011199001</v>
       </c>
       <c r="H1496" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
         </is>
       </c>
     </row>
@@ -50745,11 +50745,11 @@
         </is>
       </c>
       <c r="G1497">
-        <v>1215012102000</v>
+        <v>1215012101000</v>
       </c>
       <c r="H1497" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -50779,11 +50779,11 @@
         </is>
       </c>
       <c r="G1498">
-        <v>1215012103000</v>
+        <v>1215012102000</v>
       </c>
       <c r="H1498" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -50813,11 +50813,11 @@
         </is>
       </c>
       <c r="G1499">
-        <v>1215012104000</v>
+        <v>1215012103000</v>
       </c>
       <c r="H1499" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -50847,11 +50847,11 @@
         </is>
       </c>
       <c r="G1500">
-        <v>1215012105000</v>
+        <v>1215012104000</v>
       </c>
       <c r="H1500" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -50881,11 +50881,11 @@
         </is>
       </c>
       <c r="G1501">
-        <v>1215012106000</v>
+        <v>1215012105000</v>
       </c>
       <c r="H1501" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -50915,11 +50915,11 @@
         </is>
       </c>
       <c r="G1502">
-        <v>1215012107000</v>
+        <v>1215012106000</v>
       </c>
       <c r="H1502" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -50949,11 +50949,11 @@
         </is>
       </c>
       <c r="G1503">
-        <v>1215013101000</v>
+        <v>1215012107000</v>
       </c>
       <c r="H1503" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -50983,11 +50983,11 @@
         </is>
       </c>
       <c r="G1504">
-        <v>1215013102000</v>
+        <v>1215013101000</v>
       </c>
       <c r="H1504" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -51017,11 +51017,11 @@
         </is>
       </c>
       <c r="G1505">
-        <v>1215013104000</v>
+        <v>1215013102000</v>
       </c>
       <c r="H1505" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -51051,11 +51051,11 @@
         </is>
       </c>
       <c r="G1506">
-        <v>1215013105000</v>
+        <v>1215013104000</v>
       </c>
       <c r="H1506" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -51085,11 +51085,11 @@
         </is>
       </c>
       <c r="G1507">
-        <v>1215013106000</v>
+        <v>1215013105000</v>
       </c>
       <c r="H1507" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -51119,11 +51119,11 @@
         </is>
       </c>
       <c r="G1508">
-        <v>1215014101000</v>
+        <v>1215013106000</v>
       </c>
       <c r="H1508" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -51153,11 +51153,11 @@
         </is>
       </c>
       <c r="G1509">
-        <v>1215015101000</v>
+        <v>1215014101000</v>
       </c>
       <c r="H1509" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51179,19 +51179,19 @@
         </is>
       </c>
       <c r="E1510">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1510" t="inlineStr">
         <is>
-          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1510">
-        <v>1999030101000</v>
+        <v>1215015101000</v>
       </c>
       <c r="H1510" t="inlineStr">
         <is>
-          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51213,19 +51213,19 @@
         </is>
       </c>
       <c r="E1511">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="F1511" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1511">
-        <v>1219991399000</v>
+        <v>1999030101000</v>
       </c>
       <c r="H1511" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
+          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51255,11 +51255,11 @@
         </is>
       </c>
       <c r="G1512">
-        <v>1219991499000</v>
+        <v>1219991399000</v>
       </c>
       <c r="H1512" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
+          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -51289,11 +51289,11 @@
         </is>
       </c>
       <c r="G1513">
-        <v>1321040101000</v>
+        <v>1219991499000</v>
       </c>
       <c r="H1513" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
+          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -51323,11 +51323,11 @@
         </is>
       </c>
       <c r="G1514">
-        <v>1321040102000</v>
+        <v>1321040101000</v>
       </c>
       <c r="H1514" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
         </is>
       </c>
     </row>
@@ -51357,45 +51357,45 @@
         </is>
       </c>
       <c r="G1515">
-        <v>1922990199000</v>
+        <v>1321040102000</v>
       </c>
       <c r="H1515" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
         </is>
       </c>
     </row>
     <row r="1516">
       <c r="A1516">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1516" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1516">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1516" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1516">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F1516" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1516">
-        <v>1215521104000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1516" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -51425,11 +51425,11 @@
         </is>
       </c>
       <c r="G1517">
-        <v>1215522104000</v>
+        <v>1215521104000</v>
       </c>
       <c r="H1517" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -51459,45 +51459,45 @@
         </is>
       </c>
       <c r="G1518">
-        <v>1215523104000</v>
+        <v>1215522104000</v>
       </c>
       <c r="H1518" t="inlineStr">
         <is>
-          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1519">
       <c r="A1519">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1519" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1519">
-        <v>1301</v>
+        <v>9999</v>
       </c>
       <c r="D1519" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1519">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F1519" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1519">
-        <v>1321010101000</v>
+        <v>1215523104000</v>
       </c>
       <c r="H1519" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -51511,27 +51511,27 @@
         </is>
       </c>
       <c r="C1520">
-        <v>2371</v>
+        <v>1301</v>
       </c>
       <c r="D1520" t="inlineStr">
         <is>
-          <t>IMA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1520">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1520" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1520">
-        <v>1922990199000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1520" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51545,11 +51545,11 @@
         </is>
       </c>
       <c r="C1521">
-        <v>4291</v>
+        <v>2371</v>
       </c>
       <c r="D1521" t="inlineStr">
         <is>
-          <t>FES</t>
+          <t>IMA</t>
         </is>
       </c>
       <c r="E1521">
@@ -51579,11 +51579,11 @@
         </is>
       </c>
       <c r="C1522">
-        <v>9999</v>
+        <v>4291</v>
       </c>
       <c r="D1522" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FES</t>
         </is>
       </c>
       <c r="E1522">
@@ -51595,11 +51595,11 @@
         </is>
       </c>
       <c r="G1522">
-        <v>1321010101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1522" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -51629,11 +51629,11 @@
         </is>
       </c>
       <c r="G1523">
-        <v>2999990102000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1523" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51663,11 +51663,11 @@
         </is>
       </c>
       <c r="G1524">
-        <v>2999990103000</v>
+        <v>2999990102000</v>
       </c>
       <c r="H1524" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
         </is>
       </c>
     </row>
@@ -51681,27 +51681,27 @@
         </is>
       </c>
       <c r="C1525">
-        <v>1301</v>
+        <v>9999</v>
       </c>
       <c r="D1525" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1525">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="F1525" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
         </is>
       </c>
       <c r="G1525">
-        <v>1332040101000</v>
+        <v>2999990103000</v>
       </c>
       <c r="H1525" t="inlineStr">
         <is>
-          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
         </is>
       </c>
     </row>
@@ -51715,27 +51715,27 @@
         </is>
       </c>
       <c r="C1526">
-        <v>9999</v>
+        <v>1301</v>
       </c>
       <c r="D1526" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1526">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1526" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1526">
-        <v>1922990199000</v>
+        <v>1332040101000</v>
       </c>
       <c r="H1526" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
         </is>
       </c>
     </row>
@@ -51765,11 +51765,11 @@
         </is>
       </c>
       <c r="G1527">
-        <v>1999992199000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1527" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -51799,9 +51799,43 @@
         </is>
       </c>
       <c r="G1528">
+        <v>1999992199000</v>
+      </c>
+      <c r="H1528" t="inlineStr">
+        <is>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529">
+        <v>899</v>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1529">
+        <v>9999</v>
+      </c>
+      <c r="D1529" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1529">
+        <v>95</v>
+      </c>
+      <c r="F1529" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1529">
         <v>1921990101000</v>
       </c>
-      <c r="H1528" t="inlineStr">
+      <c r="H1529" t="inlineStr">
         <is>
           <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>

</xml_diff>

<commit_message>
Update data package at: 2024-11-12T10:34:45Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -24388,6 +24388,11 @@
       <c r="E708">
         <v>90</v>
       </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>TRANSFERENCIAS DO FUNDEB - COMPLEMENTACAO DA UNIAO - VAAR</t>
+        </is>
+      </c>
       <c r="G708">
         <v>1715520101000</v>
       </c>
@@ -24411,6 +24416,11 @@
       </c>
       <c r="E709">
         <v>90</v>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>TRANSFERENCIAS DO FUNDEB - COMPLEMENTACAO DA UNIAO - VAAR</t>
+        </is>
       </c>
       <c r="G709">
         <v>1715520101000</v>

</xml_diff>

<commit_message>
Update data package at: 2024-12-06T10:37:46Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1752"/>
+  <dimension ref="A1:H1753"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -59213,36 +59213,31 @@
     </row>
     <row r="1740">
       <c r="A1740">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1740" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1740">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1740" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1740">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F1740" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1740">
-        <v>1215521104000</v>
-      </c>
-      <c r="H1740" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
-        </is>
+        <v>7999010101000</v>
       </c>
     </row>
     <row r="1741">
@@ -59271,11 +59266,11 @@
         </is>
       </c>
       <c r="G1741">
-        <v>1215522104000</v>
+        <v>1215521104000</v>
       </c>
       <c r="H1741" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -59305,45 +59300,45 @@
         </is>
       </c>
       <c r="G1742">
-        <v>1215523104000</v>
+        <v>1215522104000</v>
       </c>
       <c r="H1742" t="inlineStr">
         <is>
-          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1743">
       <c r="A1743">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1743" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1743">
-        <v>1301</v>
+        <v>9999</v>
       </c>
       <c r="D1743" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1743">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F1743" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1743">
-        <v>1321010101000</v>
+        <v>1215523104000</v>
       </c>
       <c r="H1743" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -59357,27 +59352,27 @@
         </is>
       </c>
       <c r="C1744">
-        <v>2371</v>
+        <v>1301</v>
       </c>
       <c r="D1744" t="inlineStr">
         <is>
-          <t>IMA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1744">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1744" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1744">
-        <v>1922990199000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1744" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59391,11 +59386,11 @@
         </is>
       </c>
       <c r="C1745">
-        <v>4291</v>
+        <v>2371</v>
       </c>
       <c r="D1745" t="inlineStr">
         <is>
-          <t>FES</t>
+          <t>IMA</t>
         </is>
       </c>
       <c r="E1745">
@@ -59425,11 +59420,11 @@
         </is>
       </c>
       <c r="C1746">
-        <v>9999</v>
+        <v>4291</v>
       </c>
       <c r="D1746" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FES</t>
         </is>
       </c>
       <c r="E1746">
@@ -59441,11 +59436,11 @@
         </is>
       </c>
       <c r="G1746">
-        <v>1321010101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1746" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59475,11 +59470,11 @@
         </is>
       </c>
       <c r="G1747">
-        <v>2999990102000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1747" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59509,11 +59504,11 @@
         </is>
       </c>
       <c r="G1748">
-        <v>2999990103000</v>
+        <v>2999990102000</v>
       </c>
       <c r="H1748" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
         </is>
       </c>
     </row>
@@ -59527,27 +59522,27 @@
         </is>
       </c>
       <c r="C1749">
-        <v>1301</v>
+        <v>9999</v>
       </c>
       <c r="D1749" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1749">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="F1749" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
         </is>
       </c>
       <c r="G1749">
-        <v>1332040101000</v>
+        <v>2999990103000</v>
       </c>
       <c r="H1749" t="inlineStr">
         <is>
-          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
         </is>
       </c>
     </row>
@@ -59561,27 +59556,27 @@
         </is>
       </c>
       <c r="C1750">
-        <v>9999</v>
+        <v>1301</v>
       </c>
       <c r="D1750" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1750">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1750" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1750">
-        <v>1922990199000</v>
+        <v>1332040101000</v>
       </c>
       <c r="H1750" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59611,11 +59606,11 @@
         </is>
       </c>
       <c r="G1751">
-        <v>1999992199000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1751" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59645,9 +59640,43 @@
         </is>
       </c>
       <c r="G1752">
+        <v>1999992199000</v>
+      </c>
+      <c r="H1752" t="inlineStr">
+        <is>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1753">
+      <c r="A1753">
+        <v>899</v>
+      </c>
+      <c r="B1753" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1753">
+        <v>9999</v>
+      </c>
+      <c r="D1753" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1753">
+        <v>95</v>
+      </c>
+      <c r="F1753" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1753">
         <v>1921990101000</v>
       </c>
-      <c r="H1752" t="inlineStr">
+      <c r="H1753" t="inlineStr">
         <is>
           <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>

</xml_diff>

<commit_message>
Update data package at: 2024-12-10T10:39:03Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1753"/>
+  <dimension ref="A1:H1761"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -57939,23 +57939,23 @@
         </is>
       </c>
       <c r="C1702">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1702" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1702">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="F1702" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1702">
-        <v>7215531103000</v>
+        <v>7219991103053</v>
       </c>
     </row>
     <row r="1703">
@@ -57968,295 +57968,255 @@
         </is>
       </c>
       <c r="C1703">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1703" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1703">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="F1703" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1703">
-        <v>7215532103000</v>
+        <v>7219991103054</v>
       </c>
     </row>
     <row r="1704">
       <c r="A1704">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1704" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1704">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1704" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1704">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F1704" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1704">
-        <v>7215021101001</v>
-      </c>
-      <c r="H1704" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>7219991103055</v>
       </c>
     </row>
     <row r="1705">
       <c r="A1705">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1705" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1705">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1705" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1705">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F1705" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1705">
-        <v>7215021101002</v>
-      </c>
-      <c r="H1705" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
-        </is>
+        <v>7219991103056</v>
       </c>
     </row>
     <row r="1706">
       <c r="A1706">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1706" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1706">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1706" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1706">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F1706" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1706">
-        <v>7215021102001</v>
-      </c>
-      <c r="H1706" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>1219991103003</v>
       </c>
     </row>
     <row r="1707">
       <c r="A1707">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1707" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1707">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1707" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1707">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F1707" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1707">
-        <v>7215021103001</v>
-      </c>
-      <c r="H1707" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>1219991103004</v>
       </c>
     </row>
     <row r="1708">
       <c r="A1708">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1708" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1708">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1708" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1708">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F1708" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1708">
-        <v>7215021104001</v>
-      </c>
-      <c r="H1708" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>1219991103005</v>
       </c>
     </row>
     <row r="1709">
       <c r="A1709">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1709" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1709">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1709" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1709">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F1709" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1709">
-        <v>7215021105001</v>
-      </c>
-      <c r="H1709" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>1219991103006</v>
       </c>
     </row>
     <row r="1710">
       <c r="A1710">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1710" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1710">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1710" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1710">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1710" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1710">
-        <v>7215021106001</v>
-      </c>
-      <c r="H1710" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>7215531103000</v>
       </c>
     </row>
     <row r="1711">
       <c r="A1711">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1711" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1711">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1711" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1711">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1711" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1711">
-        <v>7215021107001</v>
-      </c>
-      <c r="H1711" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>7215532103000</v>
       </c>
     </row>
     <row r="1712">
@@ -58277,19 +58237,19 @@
         </is>
       </c>
       <c r="E1712">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1712" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1712">
-        <v>1215011101000</v>
+        <v>7215021101001</v>
       </c>
       <c r="H1712" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58311,19 +58271,19 @@
         </is>
       </c>
       <c r="E1713">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1713" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1713">
-        <v>1215011102000</v>
+        <v>7215021101002</v>
       </c>
       <c r="H1713" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
         </is>
       </c>
     </row>
@@ -58345,19 +58305,19 @@
         </is>
       </c>
       <c r="E1714">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1714" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1714">
-        <v>1215011103000</v>
+        <v>7215021102001</v>
       </c>
       <c r="H1714" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58379,19 +58339,19 @@
         </is>
       </c>
       <c r="E1715">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1715" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1715">
-        <v>1215011104000</v>
+        <v>7215021103001</v>
       </c>
       <c r="H1715" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58413,19 +58373,19 @@
         </is>
       </c>
       <c r="E1716">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1716" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1716">
-        <v>1215011105000</v>
+        <v>7215021104001</v>
       </c>
       <c r="H1716" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58447,19 +58407,19 @@
         </is>
       </c>
       <c r="E1717">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1717" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1717">
-        <v>1215011106000</v>
+        <v>7215021105001</v>
       </c>
       <c r="H1717" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58481,19 +58441,19 @@
         </is>
       </c>
       <c r="E1718">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1718" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1718">
-        <v>1215011107000</v>
+        <v>7215021106001</v>
       </c>
       <c r="H1718" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58515,19 +58475,19 @@
         </is>
       </c>
       <c r="E1719">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1719" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1719">
-        <v>1215011199001</v>
+        <v>7215021107001</v>
       </c>
       <c r="H1719" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58557,11 +58517,11 @@
         </is>
       </c>
       <c r="G1720">
-        <v>1215012101000</v>
+        <v>1215011101000</v>
       </c>
       <c r="H1720" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58591,11 +58551,11 @@
         </is>
       </c>
       <c r="G1721">
-        <v>1215012102000</v>
+        <v>1215011102000</v>
       </c>
       <c r="H1721" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58625,11 +58585,11 @@
         </is>
       </c>
       <c r="G1722">
-        <v>1215012103000</v>
+        <v>1215011103000</v>
       </c>
       <c r="H1722" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -58659,11 +58619,11 @@
         </is>
       </c>
       <c r="G1723">
-        <v>1215012104000</v>
+        <v>1215011104000</v>
       </c>
       <c r="H1723" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -58693,11 +58653,11 @@
         </is>
       </c>
       <c r="G1724">
-        <v>1215012105000</v>
+        <v>1215011105000</v>
       </c>
       <c r="H1724" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58727,11 +58687,11 @@
         </is>
       </c>
       <c r="G1725">
-        <v>1215012106000</v>
+        <v>1215011106000</v>
       </c>
       <c r="H1725" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -58761,11 +58721,11 @@
         </is>
       </c>
       <c r="G1726">
-        <v>1215012107000</v>
+        <v>1215011107000</v>
       </c>
       <c r="H1726" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -58795,11 +58755,11 @@
         </is>
       </c>
       <c r="G1727">
-        <v>1215013101000</v>
+        <v>1215011199001</v>
       </c>
       <c r="H1727" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
         </is>
       </c>
     </row>
@@ -58829,11 +58789,11 @@
         </is>
       </c>
       <c r="G1728">
-        <v>1215013102000</v>
+        <v>1215012101000</v>
       </c>
       <c r="H1728" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58863,11 +58823,11 @@
         </is>
       </c>
       <c r="G1729">
-        <v>1215013104000</v>
+        <v>1215012102000</v>
       </c>
       <c r="H1729" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58897,11 +58857,11 @@
         </is>
       </c>
       <c r="G1730">
-        <v>1215013105000</v>
+        <v>1215012103000</v>
       </c>
       <c r="H1730" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -58931,11 +58891,11 @@
         </is>
       </c>
       <c r="G1731">
-        <v>1215013106000</v>
+        <v>1215012104000</v>
       </c>
       <c r="H1731" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -58965,11 +58925,11 @@
         </is>
       </c>
       <c r="G1732">
-        <v>1215014101000</v>
+        <v>1215012105000</v>
       </c>
       <c r="H1732" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58999,11 +58959,11 @@
         </is>
       </c>
       <c r="G1733">
-        <v>1215015101000</v>
+        <v>1215012106000</v>
       </c>
       <c r="H1733" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -59025,19 +58985,19 @@
         </is>
       </c>
       <c r="E1734">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1734" t="inlineStr">
         <is>
-          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1734">
-        <v>1999030101000</v>
+        <v>1215012107000</v>
       </c>
       <c r="H1734" t="inlineStr">
         <is>
-          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -59059,19 +59019,19 @@
         </is>
       </c>
       <c r="E1735">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1735" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1735">
-        <v>1219991399000</v>
+        <v>1215013101000</v>
       </c>
       <c r="H1735" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -59093,19 +59053,19 @@
         </is>
       </c>
       <c r="E1736">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1736" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1736">
-        <v>1219991499000</v>
+        <v>1215013102000</v>
       </c>
       <c r="H1736" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -59127,19 +59087,19 @@
         </is>
       </c>
       <c r="E1737">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1737" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1737">
-        <v>1321040101000</v>
+        <v>1215013104000</v>
       </c>
       <c r="H1737" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -59161,19 +59121,19 @@
         </is>
       </c>
       <c r="E1738">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1738" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1738">
-        <v>1321040102000</v>
+        <v>1215013105000</v>
       </c>
       <c r="H1738" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -59195,19 +59155,19 @@
         </is>
       </c>
       <c r="E1739">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1739" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1739">
-        <v>1922990199000</v>
+        <v>1215013106000</v>
       </c>
       <c r="H1739" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -59229,296 +59189,296 @@
         </is>
       </c>
       <c r="E1740">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F1740" t="inlineStr">
         <is>
-          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1740">
-        <v>7999010101000</v>
+        <v>1215014101000</v>
+      </c>
+      <c r="H1740" t="inlineStr">
+        <is>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
+        </is>
       </c>
     </row>
     <row r="1741">
       <c r="A1741">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1741" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1741">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1741" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1741">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="F1741" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1741">
-        <v>1215521104000</v>
+        <v>1215015101000</v>
       </c>
       <c r="H1741" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
         </is>
       </c>
     </row>
     <row r="1742">
       <c r="A1742">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1742" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1742">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1742" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1742">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="F1742" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1742">
-        <v>1215522104000</v>
+        <v>1999030101000</v>
       </c>
       <c r="H1742" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
         </is>
       </c>
     </row>
     <row r="1743">
       <c r="A1743">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1743" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1743">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1743" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1743">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F1743" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1743">
-        <v>1215523104000</v>
+        <v>1219991399000</v>
       </c>
       <c r="H1743" t="inlineStr">
         <is>
-          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1744">
       <c r="A1744">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1744" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1744">
-        <v>1301</v>
+        <v>4711</v>
       </c>
       <c r="D1744" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1744">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1744" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1744">
-        <v>1321010101000</v>
+        <v>1219991499000</v>
       </c>
       <c r="H1744" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1745">
       <c r="A1745">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1745" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1745">
-        <v>2371</v>
+        <v>4711</v>
       </c>
       <c r="D1745" t="inlineStr">
         <is>
-          <t>IMA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1745">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="F1745" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1745">
-        <v>1922990199000</v>
+        <v>1321040101000</v>
       </c>
       <c r="H1745" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
         </is>
       </c>
     </row>
     <row r="1746">
       <c r="A1746">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1746" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1746">
-        <v>4291</v>
+        <v>4711</v>
       </c>
       <c r="D1746" t="inlineStr">
         <is>
-          <t>FES</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1746">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="F1746" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1746">
-        <v>1922990199000</v>
+        <v>1321040102000</v>
       </c>
       <c r="H1746" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
         </is>
       </c>
     </row>
     <row r="1747">
       <c r="A1747">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1747" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1747">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1747" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1747">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="F1747" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1747">
-        <v>1321010101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1747" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1748">
       <c r="A1748">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1748" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1748">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1748" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1748">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="F1748" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1748">
-        <v>2999990102000</v>
-      </c>
-      <c r="H1748" t="inlineStr">
-        <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
-        </is>
+        <v>7999010101000</v>
       </c>
     </row>
     <row r="1749">
       <c r="A1749">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1749" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1749">
@@ -59530,63 +59490,63 @@
         </is>
       </c>
       <c r="E1749">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F1749" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1749">
-        <v>2999990103000</v>
+        <v>1215521104000</v>
       </c>
       <c r="H1749" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1750">
       <c r="A1750">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1750" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1750">
-        <v>1301</v>
+        <v>9999</v>
       </c>
       <c r="D1750" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1750">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F1750" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1750">
-        <v>1332040101000</v>
+        <v>1215522104000</v>
       </c>
       <c r="H1750" t="inlineStr">
         <is>
-          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1751">
       <c r="A1751">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1751" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1751">
@@ -59598,19 +59558,19 @@
         </is>
       </c>
       <c r="E1751">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F1751" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1751">
-        <v>1922990199000</v>
+        <v>1215523104000</v>
       </c>
       <c r="H1751" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -59624,27 +59584,27 @@
         </is>
       </c>
       <c r="C1752">
-        <v>9999</v>
+        <v>1301</v>
       </c>
       <c r="D1752" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1752">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1752" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1752">
-        <v>1999992199000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1752" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59658,11 +59618,11 @@
         </is>
       </c>
       <c r="C1753">
-        <v>9999</v>
+        <v>2371</v>
       </c>
       <c r="D1753" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IMA</t>
         </is>
       </c>
       <c r="E1753">
@@ -59674,9 +59634,281 @@
         </is>
       </c>
       <c r="G1753">
+        <v>1922990199000</v>
+      </c>
+      <c r="H1753" t="inlineStr">
+        <is>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1754">
+      <c r="A1754">
+        <v>899</v>
+      </c>
+      <c r="B1754" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1754">
+        <v>4291</v>
+      </c>
+      <c r="D1754" t="inlineStr">
+        <is>
+          <t>FES</t>
+        </is>
+      </c>
+      <c r="E1754">
+        <v>95</v>
+      </c>
+      <c r="F1754" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1754">
+        <v>1922990199000</v>
+      </c>
+      <c r="H1754" t="inlineStr">
+        <is>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1755">
+      <c r="A1755">
+        <v>899</v>
+      </c>
+      <c r="B1755" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1755">
+        <v>9999</v>
+      </c>
+      <c r="D1755" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1755">
+        <v>95</v>
+      </c>
+      <c r="F1755" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1755">
+        <v>1321010101000</v>
+      </c>
+      <c r="H1755" t="inlineStr">
+        <is>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="1756">
+      <c r="A1756">
+        <v>899</v>
+      </c>
+      <c r="B1756" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1756">
+        <v>9999</v>
+      </c>
+      <c r="D1756" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1756">
+        <v>95</v>
+      </c>
+      <c r="F1756" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1756">
+        <v>2999990102000</v>
+      </c>
+      <c r="H1756" t="inlineStr">
+        <is>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1757">
+      <c r="A1757">
+        <v>899</v>
+      </c>
+      <c r="B1757" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1757">
+        <v>9999</v>
+      </c>
+      <c r="D1757" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1757">
+        <v>95</v>
+      </c>
+      <c r="F1757" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1757">
+        <v>2999990103000</v>
+      </c>
+      <c r="H1757" t="inlineStr">
+        <is>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="1758">
+      <c r="A1758">
+        <v>899</v>
+      </c>
+      <c r="B1758" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1758">
+        <v>1301</v>
+      </c>
+      <c r="D1758" t="inlineStr">
+        <is>
+          <t>SEINFRA</t>
+        </is>
+      </c>
+      <c r="E1758">
+        <v>59</v>
+      </c>
+      <c r="F1758" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="G1758">
+        <v>1332040101000</v>
+      </c>
+      <c r="H1758" t="inlineStr">
+        <is>
+          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="1759">
+      <c r="A1759">
+        <v>899</v>
+      </c>
+      <c r="B1759" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1759">
+        <v>9999</v>
+      </c>
+      <c r="D1759" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1759">
+        <v>95</v>
+      </c>
+      <c r="F1759" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1759">
+        <v>1922990199000</v>
+      </c>
+      <c r="H1759" t="inlineStr">
+        <is>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1760">
+      <c r="A1760">
+        <v>899</v>
+      </c>
+      <c r="B1760" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1760">
+        <v>9999</v>
+      </c>
+      <c r="D1760" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1760">
+        <v>95</v>
+      </c>
+      <c r="F1760" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1760">
+        <v>1999992199000</v>
+      </c>
+      <c r="H1760" t="inlineStr">
+        <is>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1761">
+      <c r="A1761">
+        <v>899</v>
+      </c>
+      <c r="B1761" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1761">
+        <v>9999</v>
+      </c>
+      <c r="D1761" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1761">
+        <v>95</v>
+      </c>
+      <c r="F1761" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1761">
         <v>1921990101000</v>
       </c>
-      <c r="H1753" t="inlineStr">
+      <c r="H1761" t="inlineStr">
         <is>
           <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
         </is>

</xml_diff>

<commit_message>
Update data package at: 2024-12-19T10:36:45Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1763"/>
+  <dimension ref="A1:H1767"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -58213,15 +58213,15 @@
         </is>
       </c>
       <c r="E1711">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="F1711" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO A APOSENTADORIA</t>
         </is>
       </c>
       <c r="G1711">
-        <v>7215531103000</v>
+        <v>1219991110001</v>
       </c>
     </row>
     <row r="1712">
@@ -58250,109 +58250,94 @@
         </is>
       </c>
       <c r="G1712">
-        <v>7215532103000</v>
+        <v>7215531103000</v>
       </c>
     </row>
     <row r="1713">
       <c r="A1713">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1713" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1713">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1713" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1713">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1713" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1713">
-        <v>7215021101001</v>
-      </c>
-      <c r="H1713" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>7215532103000</v>
       </c>
     </row>
     <row r="1714">
       <c r="A1714">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1714" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1714">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1714" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1714">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1714" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1714">
-        <v>7215021101002</v>
-      </c>
-      <c r="H1714" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
-        </is>
+        <v>7219991110051</v>
       </c>
     </row>
     <row r="1715">
       <c r="A1715">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B1715" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
         </is>
       </c>
       <c r="C1715">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1715" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1715">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1715" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1715">
-        <v>7215021102001</v>
-      </c>
-      <c r="H1715" t="inlineStr">
-        <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
-        </is>
+        <v>7219991110052</v>
       </c>
     </row>
     <row r="1716">
@@ -58381,11 +58366,11 @@
         </is>
       </c>
       <c r="G1716">
-        <v>7215021103001</v>
+        <v>7215021101001</v>
       </c>
       <c r="H1716" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58415,11 +58400,11 @@
         </is>
       </c>
       <c r="G1717">
-        <v>7215021104001</v>
+        <v>7215021101002</v>
       </c>
       <c r="H1717" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
         </is>
       </c>
     </row>
@@ -58449,11 +58434,11 @@
         </is>
       </c>
       <c r="G1718">
-        <v>7215021105001</v>
+        <v>7215021102001</v>
       </c>
       <c r="H1718" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58483,11 +58468,11 @@
         </is>
       </c>
       <c r="G1719">
-        <v>7215021106001</v>
+        <v>7215021103001</v>
       </c>
       <c r="H1719" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58517,11 +58502,11 @@
         </is>
       </c>
       <c r="G1720">
-        <v>7215021107001</v>
+        <v>7215021104001</v>
       </c>
       <c r="H1720" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58543,19 +58528,19 @@
         </is>
       </c>
       <c r="E1721">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1721" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1721">
-        <v>1215011101000</v>
+        <v>7215021105001</v>
       </c>
       <c r="H1721" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58577,19 +58562,19 @@
         </is>
       </c>
       <c r="E1722">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1722" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1722">
-        <v>1215011102000</v>
+        <v>7215021106001</v>
       </c>
       <c r="H1722" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58611,19 +58596,19 @@
         </is>
       </c>
       <c r="E1723">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1723" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1723">
-        <v>1215011103000</v>
+        <v>7215021107001</v>
       </c>
       <c r="H1723" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
         </is>
       </c>
     </row>
@@ -58653,11 +58638,11 @@
         </is>
       </c>
       <c r="G1724">
-        <v>1215011104000</v>
+        <v>1215011101000</v>
       </c>
       <c r="H1724" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58687,11 +58672,11 @@
         </is>
       </c>
       <c r="G1725">
-        <v>1215011105000</v>
+        <v>1215011102000</v>
       </c>
       <c r="H1725" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58721,11 +58706,11 @@
         </is>
       </c>
       <c r="G1726">
-        <v>1215011106000</v>
+        <v>1215011103000</v>
       </c>
       <c r="H1726" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -58755,11 +58740,11 @@
         </is>
       </c>
       <c r="G1727">
-        <v>1215011107000</v>
+        <v>1215011104000</v>
       </c>
       <c r="H1727" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -58789,11 +58774,11 @@
         </is>
       </c>
       <c r="G1728">
-        <v>1215011199001</v>
+        <v>1215011105000</v>
       </c>
       <c r="H1728" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58823,11 +58808,11 @@
         </is>
       </c>
       <c r="G1729">
-        <v>1215012101000</v>
+        <v>1215011106000</v>
       </c>
       <c r="H1729" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -58857,11 +58842,11 @@
         </is>
       </c>
       <c r="G1730">
-        <v>1215012102000</v>
+        <v>1215011107000</v>
       </c>
       <c r="H1730" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -58891,11 +58876,11 @@
         </is>
       </c>
       <c r="G1731">
-        <v>1215012103000</v>
+        <v>1215011199001</v>
       </c>
       <c r="H1731" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
         </is>
       </c>
     </row>
@@ -58925,11 +58910,11 @@
         </is>
       </c>
       <c r="G1732">
-        <v>1215012104000</v>
+        <v>1215012101000</v>
       </c>
       <c r="H1732" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58959,11 +58944,11 @@
         </is>
       </c>
       <c r="G1733">
-        <v>1215012105000</v>
+        <v>1215012102000</v>
       </c>
       <c r="H1733" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58993,11 +58978,11 @@
         </is>
       </c>
       <c r="G1734">
-        <v>1215012106000</v>
+        <v>1215012103000</v>
       </c>
       <c r="H1734" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -59027,11 +59012,11 @@
         </is>
       </c>
       <c r="G1735">
-        <v>1215012107000</v>
+        <v>1215012104000</v>
       </c>
       <c r="H1735" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -59061,11 +59046,11 @@
         </is>
       </c>
       <c r="G1736">
-        <v>1215013101000</v>
+        <v>1215012105000</v>
       </c>
       <c r="H1736" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -59095,11 +59080,11 @@
         </is>
       </c>
       <c r="G1737">
-        <v>1215013102000</v>
+        <v>1215012106000</v>
       </c>
       <c r="H1737" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -59129,11 +59114,11 @@
         </is>
       </c>
       <c r="G1738">
-        <v>1215013104000</v>
+        <v>1215012107000</v>
       </c>
       <c r="H1738" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -59163,11 +59148,11 @@
         </is>
       </c>
       <c r="G1739">
-        <v>1215013105000</v>
+        <v>1215013101000</v>
       </c>
       <c r="H1739" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -59197,11 +59182,11 @@
         </is>
       </c>
       <c r="G1740">
-        <v>1215013106000</v>
+        <v>1215013102000</v>
       </c>
       <c r="H1740" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -59231,11 +59216,11 @@
         </is>
       </c>
       <c r="G1741">
-        <v>1215014101000</v>
+        <v>1215013104000</v>
       </c>
       <c r="H1741" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -59265,11 +59250,11 @@
         </is>
       </c>
       <c r="G1742">
-        <v>1215015101000</v>
+        <v>1215013105000</v>
       </c>
       <c r="H1742" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -59291,19 +59276,19 @@
         </is>
       </c>
       <c r="E1743">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1743" t="inlineStr">
         <is>
-          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1743">
-        <v>1999030101000</v>
+        <v>1215013106000</v>
       </c>
       <c r="H1743" t="inlineStr">
         <is>
-          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -59325,19 +59310,19 @@
         </is>
       </c>
       <c r="E1744">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1744" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1744">
-        <v>1219991399000</v>
+        <v>1215014101000</v>
       </c>
       <c r="H1744" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59359,19 +59344,19 @@
         </is>
       </c>
       <c r="E1745">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1745" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1745">
-        <v>1219991499000</v>
+        <v>1215015101000</v>
       </c>
       <c r="H1745" t="inlineStr">
         <is>
-          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59393,19 +59378,19 @@
         </is>
       </c>
       <c r="E1746">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="F1746" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1746">
-        <v>1321040101000</v>
+        <v>1999030101000</v>
       </c>
       <c r="H1746" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
+          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59435,11 +59420,11 @@
         </is>
       </c>
       <c r="G1747">
-        <v>1321040102000</v>
+        <v>1219991399000</v>
       </c>
       <c r="H1747" t="inlineStr">
         <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
+          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59469,11 +59454,11 @@
         </is>
       </c>
       <c r="G1748">
-        <v>1922990199000</v>
+        <v>1219991499000</v>
       </c>
       <c r="H1748" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59495,228 +59480,223 @@
         </is>
       </c>
       <c r="E1749">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F1749" t="inlineStr">
         <is>
-          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1749">
-        <v>7999010101000</v>
+        <v>1321040101000</v>
+      </c>
+      <c r="H1749" t="inlineStr">
+        <is>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
+        </is>
       </c>
     </row>
     <row r="1750">
       <c r="A1750">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1750" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1750">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1750" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1750">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F1750" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1750">
-        <v>1215521104000</v>
+        <v>1321040102000</v>
       </c>
       <c r="H1750" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
         </is>
       </c>
     </row>
     <row r="1751">
       <c r="A1751">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1751" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1751">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1751" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1751">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F1751" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1751">
-        <v>1215522104000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1751" t="inlineStr">
         <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
     <row r="1752">
       <c r="A1752">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B1752" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1752">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1752" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1752">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F1752" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1752">
-        <v>1215523104000</v>
-      </c>
-      <c r="H1752" t="inlineStr">
-        <is>
-          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
-        </is>
+        <v>7999010101000</v>
       </c>
     </row>
     <row r="1753">
       <c r="A1753">
-        <v>899</v>
+        <v>801</v>
       </c>
       <c r="B1753" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1753">
-        <v>1301</v>
+        <v>4711</v>
       </c>
       <c r="D1753" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1753">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1753" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1753">
-        <v>1321010101000</v>
-      </c>
-      <c r="H1753" t="inlineStr">
-        <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
-        </is>
+        <v>7999992114001</v>
       </c>
     </row>
     <row r="1754">
       <c r="A1754">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1754" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1754">
-        <v>2371</v>
+        <v>9999</v>
       </c>
       <c r="D1754" t="inlineStr">
         <is>
-          <t>IMA</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1754">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F1754" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1754">
-        <v>1922990199000</v>
+        <v>1215521104000</v>
       </c>
       <c r="H1754" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1755">
       <c r="A1755">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1755" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1755">
-        <v>4291</v>
+        <v>9999</v>
       </c>
       <c r="D1755" t="inlineStr">
         <is>
-          <t>FES</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1755">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F1755" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1755">
-        <v>1922990199000</v>
+        <v>1215522104000</v>
       </c>
       <c r="H1755" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1756">
       <c r="A1756">
-        <v>899</v>
+        <v>803</v>
       </c>
       <c r="B1756" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1756">
@@ -59728,19 +59708,19 @@
         </is>
       </c>
       <c r="E1756">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F1756" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1756">
-        <v>1321010101000</v>
+        <v>1215523104000</v>
       </c>
       <c r="H1756" t="inlineStr">
         <is>
-          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
+          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
@@ -59754,27 +59734,27 @@
         </is>
       </c>
       <c r="C1757">
-        <v>9999</v>
+        <v>1301</v>
       </c>
       <c r="D1757" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1757">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="F1757" t="inlineStr">
         <is>
-          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+          <t>OUTROS RECURSOS VINCULADOS</t>
         </is>
       </c>
       <c r="G1757">
-        <v>2999990102000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1757" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59788,11 +59768,11 @@
         </is>
       </c>
       <c r="C1758">
-        <v>9999</v>
+        <v>2371</v>
       </c>
       <c r="D1758" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IMA</t>
         </is>
       </c>
       <c r="E1758">
@@ -59804,11 +59784,11 @@
         </is>
       </c>
       <c r="G1758">
-        <v>2999990103000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1758" t="inlineStr">
         <is>
-          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59822,27 +59802,27 @@
         </is>
       </c>
       <c r="C1759">
-        <v>1301</v>
+        <v>4291</v>
       </c>
       <c r="D1759" t="inlineStr">
         <is>
-          <t>SEINFRA</t>
+          <t>FES</t>
         </is>
       </c>
       <c r="E1759">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="F1759" t="inlineStr">
         <is>
-          <t>OUTROS RECURSOS VINCULADOS</t>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
         </is>
       </c>
       <c r="G1759">
-        <v>1332040101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1759" t="inlineStr">
         <is>
-          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59872,11 +59852,11 @@
         </is>
       </c>
       <c r="G1760">
-        <v>1922990199000</v>
+        <v>1321010101000</v>
       </c>
       <c r="H1760" t="inlineStr">
         <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+          <t>REMUNERACAO DEPOSITOS BANCARIOS - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59906,11 +59886,11 @@
         </is>
       </c>
       <c r="G1761">
-        <v>1999992199000</v>
+        <v>2999990102000</v>
       </c>
       <c r="H1761" t="inlineStr">
         <is>
-          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DA MINA DO CORREGO DO FEIJAO EM BRUMADINHO</t>
         </is>
       </c>
     </row>
@@ -59940,11 +59920,11 @@
         </is>
       </c>
       <c r="G1762">
-        <v>1921990101000</v>
+        <v>2999990103000</v>
       </c>
       <c r="H1762" t="inlineStr">
         <is>
-          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
+          <t>DEMAIS REC. CAPITAL - PRINC. - ROMPIMENTO DA BARRAGEM DE FUNDAO EM MARIANA - RENOVA</t>
         </is>
       </c>
     </row>
@@ -59958,22 +59938,158 @@
         </is>
       </c>
       <c r="C1763">
-        <v>9999</v>
+        <v>1301</v>
       </c>
       <c r="D1763" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>SEINFRA</t>
         </is>
       </c>
       <c r="E1763">
+        <v>59</v>
+      </c>
+      <c r="F1763" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="G1763">
+        <v>1332040101000</v>
+      </c>
+      <c r="H1763" t="inlineStr">
+        <is>
+          <t>DELEG. EXPLORACAO INFRAEST. AEROPORTUARIA - PRINC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="1764">
+      <c r="A1764">
+        <v>899</v>
+      </c>
+      <c r="B1764" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1764">
+        <v>9999</v>
+      </c>
+      <c r="D1764" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1764">
+        <v>95</v>
+      </c>
+      <c r="F1764" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1764">
+        <v>1922990199000</v>
+      </c>
+      <c r="H1764" t="inlineStr">
+        <is>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1765">
+      <c r="A1765">
+        <v>899</v>
+      </c>
+      <c r="B1765" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1765">
+        <v>9999</v>
+      </c>
+      <c r="D1765" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1765">
+        <v>95</v>
+      </c>
+      <c r="F1765" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1765">
+        <v>1999992199000</v>
+      </c>
+      <c r="H1765" t="inlineStr">
+        <is>
+          <t>OUTRAS REC. - PRIMARIAS - PRINC. - DEMAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1766">
+      <c r="A1766">
+        <v>899</v>
+      </c>
+      <c r="B1766" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1766">
+        <v>9999</v>
+      </c>
+      <c r="D1766" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1766">
+        <v>95</v>
+      </c>
+      <c r="F1766" t="inlineStr">
+        <is>
+          <t>RECURSOS RECEBIDOS POR DANOS ADVINDOS DE DESASTRES SOCIOAMBIENTAIS</t>
+        </is>
+      </c>
+      <c r="G1766">
+        <v>1921990101000</v>
+      </c>
+      <c r="H1766" t="inlineStr">
+        <is>
+          <t>OUTRAS INDENIZACOES - PRINC. - IMPACTOS E DANOS AMBIENTAIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="1767">
+      <c r="A1767">
+        <v>899</v>
+      </c>
+      <c r="B1767" t="inlineStr">
+        <is>
+          <t>OUTROS RECURSOS VINCULADOS</t>
+        </is>
+      </c>
+      <c r="C1767">
+        <v>9999</v>
+      </c>
+      <c r="D1767" t="inlineStr">
+        <is>
+          <t>EMG - ADM. DIRETA</t>
+        </is>
+      </c>
+      <c r="E1767">
         <v>80</v>
       </c>
-      <c r="F1763" t="inlineStr">
+      <c r="F1767" t="inlineStr">
         <is>
           <t>RECURSOS DO ACORDO DE REPACTUACAO DO RIO DOCE</t>
         </is>
       </c>
-      <c r="G1763">
+      <c r="G1767">
         <v>2999990104000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data package at: 2024-12-27T10:33:31Z
</commit_message>
<xml_diff>
--- a/data/matriz_receita_desc.xlsx
+++ b/data/matriz_receita_desc.xlsx
@@ -57920,23 +57920,23 @@
         </is>
       </c>
       <c r="C1701">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1701" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1701">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F1701" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO A APOSENTADORIA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1701">
-        <v>1215521101000</v>
+        <v>7219991103053</v>
       </c>
     </row>
     <row r="1702">
@@ -57949,23 +57949,23 @@
         </is>
       </c>
       <c r="C1702">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1702" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1702">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="F1702" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1702">
-        <v>7215531102000</v>
+        <v>7219991103054</v>
       </c>
     </row>
     <row r="1703">
@@ -57978,23 +57978,23 @@
         </is>
       </c>
       <c r="C1703">
-        <v>9999</v>
+        <v>2121</v>
       </c>
       <c r="D1703" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1703">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F1703" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1703">
-        <v>7215532102000</v>
+        <v>1219991103003</v>
       </c>
     </row>
     <row r="1704">
@@ -58015,363 +58015,423 @@
         </is>
       </c>
       <c r="E1704">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1704" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1704">
-        <v>7219991103053</v>
+        <v>1219991103004</v>
       </c>
     </row>
     <row r="1705">
       <c r="A1705">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1705" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1705">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1705" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1705">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F1705" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1705">
-        <v>7219991103054</v>
+        <v>7215021101001</v>
+      </c>
+      <c r="H1705" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1706">
       <c r="A1706">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1706" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1706">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1706" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1706">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F1706" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1706">
-        <v>7219991103055</v>
+        <v>7215021101002</v>
+      </c>
+      <c r="H1706" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
+        </is>
       </c>
     </row>
     <row r="1707">
       <c r="A1707">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1707" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1707">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1707" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1707">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F1707" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1707">
-        <v>7219991103056</v>
+        <v>7215021102001</v>
+      </c>
+      <c r="H1707" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1708">
       <c r="A1708">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1708" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1708">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1708" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1708">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F1708" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1708">
-        <v>1219991103003</v>
+        <v>7215021103001</v>
+      </c>
+      <c r="H1708" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1709">
       <c r="A1709">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1709" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1709">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1709" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1709">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F1709" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1709">
-        <v>1219991103004</v>
+        <v>7215021104001</v>
+      </c>
+      <c r="H1709" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1710">
       <c r="A1710">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1710" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1710">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1710" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1710">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F1710" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1710">
-        <v>1219991103005</v>
+        <v>7215021105001</v>
+      </c>
+      <c r="H1710" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1711">
       <c r="A1711">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1711" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1711">
-        <v>2121</v>
+        <v>4711</v>
       </c>
       <c r="D1711" t="inlineStr">
         <is>
-          <t>IPSM</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1711">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F1711" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1711">
-        <v>1219991103006</v>
+        <v>7215021106001</v>
+      </c>
+      <c r="H1711" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1712">
       <c r="A1712">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1712" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1712">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1712" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1712">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F1712" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO A APOSENTADORIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
         </is>
       </c>
       <c r="G1712">
-        <v>1219991110001</v>
+        <v>7215021107001</v>
+      </c>
+      <c r="H1712" t="inlineStr">
+        <is>
+          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
+        </is>
       </c>
     </row>
     <row r="1713">
       <c r="A1713">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1713" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1713">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1713" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1713">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="F1713" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1713">
-        <v>7215531103000</v>
+        <v>1215011101000</v>
+      </c>
+      <c r="H1713" t="inlineStr">
+        <is>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
+        </is>
       </c>
     </row>
     <row r="1714">
       <c r="A1714">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1714" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1714">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1714" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1714">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="F1714" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1714">
-        <v>7215532103000</v>
+        <v>1215011102000</v>
+      </c>
+      <c r="H1714" t="inlineStr">
+        <is>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+        </is>
       </c>
     </row>
     <row r="1715">
       <c r="A1715">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1715" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1715">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1715" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1715">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="F1715" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1715">
-        <v>7219991110051</v>
+        <v>1215011103000</v>
+      </c>
+      <c r="H1715" t="inlineStr">
+        <is>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+        </is>
       </c>
     </row>
     <row r="1716">
       <c r="A1716">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B1716" t="inlineStr">
         <is>
-          <t>OUTRAS VINCULAÇÕES LEGAIS</t>
+          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
         </is>
       </c>
       <c r="C1716">
-        <v>9999</v>
+        <v>4711</v>
       </c>
       <c r="D1716" t="inlineStr">
         <is>
-          <t>EMG - ADM. DIRETA</t>
+          <t>FFP - MG</t>
         </is>
       </c>
       <c r="E1716">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="F1716" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1716">
-        <v>7219991110052</v>
+        <v>1215011104000</v>
+      </c>
+      <c r="H1716" t="inlineStr">
+        <is>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+        </is>
       </c>
     </row>
     <row r="1717">
@@ -58392,19 +58452,19 @@
         </is>
       </c>
       <c r="E1717">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1717" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1717">
-        <v>7215021101001</v>
+        <v>1215011105000</v>
       </c>
       <c r="H1717" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58426,19 +58486,19 @@
         </is>
       </c>
       <c r="E1718">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1718" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1718">
-        <v>7215021101002</v>
+        <v>1215011106000</v>
       </c>
       <c r="H1718" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - EXECUTIVO - CONTRIB. SUPLEMENTAR</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -58460,19 +58520,19 @@
         </is>
       </c>
       <c r="E1719">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1719" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1719">
-        <v>7215021102001</v>
+        <v>1215011107000</v>
       </c>
       <c r="H1719" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - ALMG - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -58494,19 +58554,19 @@
         </is>
       </c>
       <c r="E1720">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1720" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1720">
-        <v>7215021103001</v>
+        <v>1215011199001</v>
       </c>
       <c r="H1720" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TCEMG - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
         </is>
       </c>
     </row>
@@ -58528,19 +58588,19 @@
         </is>
       </c>
       <c r="E1721">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1721" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1721">
-        <v>7215021104001</v>
+        <v>1215012101000</v>
       </c>
       <c r="H1721" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMG - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58562,19 +58622,19 @@
         </is>
       </c>
       <c r="E1722">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1722" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1722">
-        <v>7215021105001</v>
+        <v>1215012102000</v>
       </c>
       <c r="H1722" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - TJMMG - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58596,19 +58656,19 @@
         </is>
       </c>
       <c r="E1723">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1723" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1723">
-        <v>7215021106001</v>
+        <v>1215012103000</v>
       </c>
       <c r="H1723" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - MPMG - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
         </is>
       </c>
     </row>
@@ -58630,19 +58690,19 @@
         </is>
       </c>
       <c r="E1724">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1724" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO PATRONAL PARA O RPPS</t>
+          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
         </is>
       </c>
       <c r="G1724">
-        <v>7215021107001</v>
+        <v>1215012104000</v>
       </c>
       <c r="H1724" t="inlineStr">
         <is>
-          <t>REC. INTRA. - CONTRIB. PATRON. - SERV. CIVIL ATIVO - PRINC. - DEFPUB - CONTRIB. ORDINARIA</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -58672,11 +58732,11 @@
         </is>
       </c>
       <c r="G1725">
-        <v>1215011101000</v>
+        <v>1215012105000</v>
       </c>
       <c r="H1725" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58706,11 +58766,11 @@
         </is>
       </c>
       <c r="G1726">
-        <v>1215011102000</v>
+        <v>1215012106000</v>
       </c>
       <c r="H1726" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -58740,11 +58800,11 @@
         </is>
       </c>
       <c r="G1727">
-        <v>1215011103000</v>
+        <v>1215012107000</v>
       </c>
       <c r="H1727" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
         </is>
       </c>
     </row>
@@ -58774,11 +58834,11 @@
         </is>
       </c>
       <c r="G1728">
-        <v>1215011104000</v>
+        <v>1215013101000</v>
       </c>
       <c r="H1728" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
         </is>
       </c>
     </row>
@@ -58808,11 +58868,11 @@
         </is>
       </c>
       <c r="G1729">
-        <v>1215011105000</v>
+        <v>1215013102000</v>
       </c>
       <c r="H1729" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
         </is>
       </c>
     </row>
@@ -58842,11 +58902,11 @@
         </is>
       </c>
       <c r="G1730">
-        <v>1215011106000</v>
+        <v>1215013104000</v>
       </c>
       <c r="H1730" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
         </is>
       </c>
     </row>
@@ -58876,11 +58936,11 @@
         </is>
       </c>
       <c r="G1731">
-        <v>1215011107000</v>
+        <v>1215013105000</v>
       </c>
       <c r="H1731" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
         </is>
       </c>
     </row>
@@ -58910,11 +58970,11 @@
         </is>
       </c>
       <c r="G1732">
-        <v>1215011199001</v>
+        <v>1215013106000</v>
       </c>
       <c r="H1732" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL ATIVO - PRINC. - DEMAIS - PESSOAL LICENCIADO/A DISPOSICAO</t>
+          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
         </is>
       </c>
     </row>
@@ -58944,11 +59004,11 @@
         </is>
       </c>
       <c r="G1733">
-        <v>1215012101000</v>
+        <v>1215014101000</v>
       </c>
       <c r="H1733" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - PODER EXECUTIVO</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -58978,11 +59038,11 @@
         </is>
       </c>
       <c r="G1734">
-        <v>1215012102000</v>
+        <v>1215015101000</v>
       </c>
       <c r="H1734" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
+          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59004,19 +59064,19 @@
         </is>
       </c>
       <c r="E1735">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1735" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1735">
-        <v>1215012103000</v>
+        <v>1999030101000</v>
       </c>
       <c r="H1735" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS - TCEMG</t>
+          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
         </is>
       </c>
     </row>
@@ -59038,19 +59098,19 @@
         </is>
       </c>
       <c r="E1736">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F1736" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1736">
-        <v>1215012104000</v>
+        <v>1219991399000</v>
       </c>
       <c r="H1736" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
+          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59072,19 +59132,19 @@
         </is>
       </c>
       <c r="E1737">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F1737" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1737">
-        <v>1215012105000</v>
+        <v>1219991499000</v>
       </c>
       <c r="H1737" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59106,19 +59166,19 @@
         </is>
       </c>
       <c r="E1738">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F1738" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1738">
-        <v>1215012106000</v>
+        <v>1321040101000</v>
       </c>
       <c r="H1738" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
         </is>
       </c>
     </row>
@@ -59140,19 +59200,19 @@
         </is>
       </c>
       <c r="E1739">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F1739" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1739">
-        <v>1215012107000</v>
+        <v>1321040102000</v>
       </c>
       <c r="H1739" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL INATIVO - PRINC. - DEFENSORIA PUBLICA DO ESTADO DE MINAS GERAIS - DEFPUB</t>
+          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
         </is>
       </c>
     </row>
@@ -59174,19 +59234,19 @@
         </is>
       </c>
       <c r="E1740">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F1740" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
         </is>
       </c>
       <c r="G1740">
-        <v>1215013101000</v>
+        <v>1922990199000</v>
       </c>
       <c r="H1740" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - PODER EXECUTIVO</t>
+          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
         </is>
       </c>
     </row>
@@ -59208,20 +59268,15 @@
         </is>
       </c>
       <c r="E1741">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F1741" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1741">
-        <v>1215013102000</v>
-      </c>
-      <c r="H1741" t="inlineStr">
-        <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - ASSEMBLEIA LEGISLATIVA DO ESTADO DE MINAS GERAIS - ALMG</t>
-        </is>
+        <v>7999010101000</v>
       </c>
     </row>
     <row r="1742">
@@ -59242,428 +59297,338 @@
         </is>
       </c>
       <c r="E1742">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F1742" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
         </is>
       </c>
       <c r="G1742">
-        <v>1215013104000</v>
-      </c>
-      <c r="H1742" t="inlineStr">
-        <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA DO ESTADO DE MINAS GERAIS - TJMG</t>
-        </is>
+        <v>7999992114001</v>
       </c>
     </row>
     <row r="1743">
       <c r="A1743">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B1743" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1743">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1743" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1743">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F1743" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1743">
-        <v>1215013105000</v>
+        <v>1215521104000</v>
       </c>
       <c r="H1743" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - TRIBUNAL DE JUSTICA MILITAR DO ESTADO DE MINAS GERAIS - TJMMG</t>
+          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1744">
       <c r="A1744">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B1744" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1744">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1744" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1744">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F1744" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1744">
-        <v>1215013106000</v>
+        <v>1215522104000</v>
       </c>
       <c r="H1744" t="inlineStr">
         <is>
-          <t>CONTRIB. SERV. CIVIL - PENSIONISTAS - PRINC. - MINISTERIO PUBLICO DO ESTADO DE MINAS GERAIS - MPMG</t>
+          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1745">
       <c r="A1745">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B1745" t="inlineStr">
         <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
+          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
         </is>
       </c>
       <c r="C1745">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1745" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1745">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F1745" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
       <c r="G1745">
-        <v>1215014101000</v>
+        <v>1215523104000</v>
       </c>
       <c r="H1745" t="inlineStr">
         <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL ATIVO - PRINC.</t>
+          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
         </is>
       </c>
     </row>
     <row r="1746">
       <c r="A1746">
-        <v>801</v>
-      </c>
-      <c r="B1746" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1746">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1746" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1746">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F1746" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO DO SERVIDOR PARA O RPPS</t>
+          <t>CONTRIBUICAO A APOSENTADORIA</t>
         </is>
       </c>
       <c r="G1746">
-        <v>1215015101000</v>
-      </c>
-      <c r="H1746" t="inlineStr">
-        <is>
-          <t>CONTRIB. ORIUNDA SENT. JUDIC. - SERV. CIVIL INATIVO - PRINC.</t>
-        </is>
+        <v>1215521101000</v>
       </c>
     </row>
     <row r="1747">
       <c r="A1747">
-        <v>801</v>
-      </c>
-      <c r="B1747" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1747">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1747" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1747">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F1747" t="inlineStr">
         <is>
-          <t>COMPENSACAO FINANCEIRA ENTRE REGIMES DE PREVIDENCIA</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1747">
-        <v>1999030101000</v>
-      </c>
-      <c r="H1747" t="inlineStr">
-        <is>
-          <t>COMPENSACOES FINANCEIRAS RGPS RPPS SIST. PROTECAO SOCIAL - PRINC.</t>
-        </is>
+        <v>7215531102000</v>
       </c>
     </row>
     <row r="1748">
       <c r="A1748">
-        <v>801</v>
-      </c>
-      <c r="B1748" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1748">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1748" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1748">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F1748" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1748">
-        <v>1219991399000</v>
-      </c>
-      <c r="H1748" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - DA - DEMAIS</t>
-        </is>
+        <v>7215532102000</v>
       </c>
     </row>
     <row r="1749">
       <c r="A1749">
-        <v>801</v>
-      </c>
-      <c r="B1749" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1749">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1749" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1749">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F1749" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1749">
-        <v>1219991499000</v>
-      </c>
-      <c r="H1749" t="inlineStr">
-        <is>
-          <t>DEMAIS CONTRIB. SOC. - DA-MJM - DEMAIS</t>
-        </is>
+        <v>7219991103055</v>
       </c>
     </row>
     <row r="1750">
       <c r="A1750">
-        <v>801</v>
-      </c>
-      <c r="B1750" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1750">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1750" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1750">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F1750" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO PATRONAL DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1750">
-        <v>1321040101000</v>
-      </c>
-      <c r="H1750" t="inlineStr">
-        <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA FIXA</t>
-        </is>
+        <v>7219991103056</v>
       </c>
     </row>
     <row r="1751">
       <c r="A1751">
-        <v>801</v>
-      </c>
-      <c r="B1751" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1751">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1751" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1751">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F1751" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1751">
-        <v>1321040102000</v>
-      </c>
-      <c r="H1751" t="inlineStr">
-        <is>
-          <t>REMUNERACAO RECURSOS RPPS - PRINC. - RENDA VARIAVEL</t>
-        </is>
+        <v>1219991103005</v>
       </c>
     </row>
     <row r="1752">
       <c r="A1752">
-        <v>801</v>
-      </c>
-      <c r="B1752" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1752">
-        <v>4711</v>
+        <v>2121</v>
       </c>
       <c r="D1752" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>IPSM</t>
         </is>
       </c>
       <c r="E1752">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F1752" t="inlineStr">
         <is>
-          <t>RECURSOS DIRETAMENTE ARRECADADOS COM VINCULACAO ESPECIFICA</t>
+          <t>CONTRIBUICAO DO SERVIDOR DO ESTADO AOS INSTITUTOS DE PREVIDENCIA</t>
         </is>
       </c>
       <c r="G1752">
-        <v>1922990199000</v>
-      </c>
-      <c r="H1752" t="inlineStr">
-        <is>
-          <t>OUTRAS RESTITUICOES - PRINC. - DEMAIS</t>
-        </is>
+        <v>1219991103006</v>
       </c>
     </row>
     <row r="1753">
       <c r="A1753">
-        <v>801</v>
-      </c>
-      <c r="B1753" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1753">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1753" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1753">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="F1753" t="inlineStr">
         <is>
-          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
+          <t>CONTRIBUICAO A APOSENTADORIA</t>
         </is>
       </c>
       <c r="G1753">
-        <v>7999010101000</v>
+        <v>1219991110001</v>
       </c>
     </row>
     <row r="1754">
       <c r="A1754">
-        <v>801</v>
-      </c>
-      <c r="B1754" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO RPPS - FUNDO EM REPARTIÇÃO (PLANO FINANCEIRO)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1754">
-        <v>4711</v>
+        <v>9999</v>
       </c>
       <c r="D1754" t="inlineStr">
         <is>
-          <t>FFP - MG</t>
+          <t>EMG - ADM. DIRETA</t>
         </is>
       </c>
       <c r="E1754">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F1754" t="inlineStr">
         <is>
-          <t>RECURSOS PARA COBERTURA DE INSUFICIENCIA FINANCEIRA DO RPPS</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1754">
-        <v>7999992114001</v>
+        <v>7215531103000</v>
       </c>
     </row>
     <row r="1755">
       <c r="A1755">
-        <v>803</v>
-      </c>
-      <c r="B1755" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1755">
         <v>9999</v>
@@ -59674,30 +59639,20 @@
         </is>
       </c>
       <c r="E1755">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1755" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1755">
-        <v>1215521104000</v>
-      </c>
-      <c r="H1755" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR ATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
-        </is>
+        <v>7215532103000</v>
       </c>
     </row>
     <row r="1756">
       <c r="A1756">
-        <v>803</v>
-      </c>
-      <c r="B1756" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1756">
         <v>9999</v>
@@ -59708,30 +59663,20 @@
         </is>
       </c>
       <c r="E1756">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1756" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1756">
-        <v>1215522104000</v>
-      </c>
-      <c r="H1756" t="inlineStr">
-        <is>
-          <t>CONTRIB. MILITAR INATIVO - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
-        </is>
+        <v>7219991110051</v>
       </c>
     </row>
     <row r="1757">
       <c r="A1757">
-        <v>803</v>
-      </c>
-      <c r="B1757" t="inlineStr">
-        <is>
-          <t>RECURSOS VINCULADOS AO SISTEMA DE PROTEÇÃO SOCIAL DOS MILITARES (SPSM)</t>
-        </is>
+        <v>804</v>
       </c>
       <c r="C1757">
         <v>9999</v>
@@ -59742,20 +59687,15 @@
         </is>
       </c>
       <c r="E1757">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1757" t="inlineStr">
         <is>
-          <t>CONTRIBUICAO MILITAR PARA CUSTEIO DO SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
+          <t>CONTRIBUICAO PATRONAL PARA CUSTEIO DOS PROVENTOS DOS MILITARES</t>
         </is>
       </c>
       <c r="G1757">
-        <v>1215523104000</v>
-      </c>
-      <c r="H1757" t="inlineStr">
-        <is>
-          <t>CONTRIB. PENSIONISTAS MILITARES - PRINC. - SISTEMA DE PROTECAO SOCIAL DOS MILITARES</t>
-        </is>
+        <v>7219991110052</v>
       </c>
     </row>
     <row r="1758">

</xml_diff>